<commit_message>
check solog size ...
</commit_message>
<xml_diff>
--- a/database/data_Project_VVIP_Final.xlsx
+++ b/database/data_Project_VVIP_Final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5112"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5112" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4106" uniqueCount="1609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4106" uniqueCount="1607">
   <si>
     <t>Tee Tele Bear</t>
   </si>
@@ -4818,33 +4818,6 @@
     <t>z5404487280405_cd2f69aafada3d2ed353b49b0d6ae01217147288311714728831</t>
   </si>
   <si>
-    <t xml:space="preserve"> S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  L</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  XL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  2XL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  3XL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Freesize</t>
-  </si>
-  <si>
     <t>productStock</t>
   </si>
   <si>
@@ -4852,6 +4825,27 @@
   </si>
   <si>
     <t>productImagesLarge</t>
+  </si>
+  <si>
+    <t>colorId</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>2XL</t>
+  </si>
+  <si>
+    <t>3XL</t>
   </si>
 </sst>
 </file>
@@ -5311,7 +5305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -5360,10 +5354,10 @@
         <v>185</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>1607</v>
+        <v>1598</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>1608</v>
+        <v>1599</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>187</v>
@@ -20540,8 +20534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -20556,13 +20550,13 @@
         <v>181</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>669</v>
+        <v>1600</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>186</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>1606</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -20573,7 +20567,7 @@
         <v>635</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -20587,7 +20581,7 @@
         <v>635</v>
       </c>
       <c r="C3" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -20601,7 +20595,7 @@
         <v>635</v>
       </c>
       <c r="C4" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -20615,7 +20609,7 @@
         <v>634</v>
       </c>
       <c r="C5" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -20629,7 +20623,7 @@
         <v>634</v>
       </c>
       <c r="C6" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -20643,7 +20637,7 @@
         <v>634</v>
       </c>
       <c r="C7" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -20657,7 +20651,7 @@
         <v>633</v>
       </c>
       <c r="C8" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -20671,7 +20665,7 @@
         <v>633</v>
       </c>
       <c r="C9" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -20685,7 +20679,7 @@
         <v>633</v>
       </c>
       <c r="C10" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D10">
         <v>50</v>
@@ -20699,7 +20693,7 @@
         <v>632</v>
       </c>
       <c r="C11" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -20713,7 +20707,7 @@
         <v>632</v>
       </c>
       <c r="C12" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D12">
         <v>50</v>
@@ -20727,7 +20721,7 @@
         <v>632</v>
       </c>
       <c r="C13" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D13">
         <v>50</v>
@@ -20741,7 +20735,7 @@
         <v>631</v>
       </c>
       <c r="C14" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D14">
         <v>50</v>
@@ -20755,7 +20749,7 @@
         <v>631</v>
       </c>
       <c r="C15" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D15">
         <v>50</v>
@@ -20769,7 +20763,7 @@
         <v>631</v>
       </c>
       <c r="C16" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D16">
         <v>50</v>
@@ -20783,7 +20777,7 @@
         <v>631</v>
       </c>
       <c r="C17" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D17">
         <v>50</v>
@@ -20797,7 +20791,7 @@
         <v>616</v>
       </c>
       <c r="C18" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D18">
         <v>50</v>
@@ -20811,7 +20805,7 @@
         <v>616</v>
       </c>
       <c r="C19" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D19">
         <v>50</v>
@@ -20825,7 +20819,7 @@
         <v>616</v>
       </c>
       <c r="C20" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D20">
         <v>50</v>
@@ -20839,7 +20833,7 @@
         <v>616</v>
       </c>
       <c r="C21" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D21">
         <v>50</v>
@@ -20853,7 +20847,7 @@
         <v>629</v>
       </c>
       <c r="C22" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D22">
         <v>50</v>
@@ -20867,7 +20861,7 @@
         <v>629</v>
       </c>
       <c r="C23" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D23">
         <v>50</v>
@@ -20881,7 +20875,7 @@
         <v>629</v>
       </c>
       <c r="C24" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D24">
         <v>50</v>
@@ -20895,7 +20889,7 @@
         <v>629</v>
       </c>
       <c r="C25" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D25">
         <v>50</v>
@@ -20909,7 +20903,7 @@
         <v>630</v>
       </c>
       <c r="C26" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D26">
         <v>50</v>
@@ -20923,7 +20917,7 @@
         <v>630</v>
       </c>
       <c r="C27" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D27">
         <v>50</v>
@@ -20937,7 +20931,7 @@
         <v>630</v>
       </c>
       <c r="C28" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D28">
         <v>50</v>
@@ -20951,7 +20945,7 @@
         <v>630</v>
       </c>
       <c r="C29" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D29">
         <v>50</v>
@@ -20965,7 +20959,7 @@
         <v>628</v>
       </c>
       <c r="C30" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D30">
         <v>50</v>
@@ -20979,7 +20973,7 @@
         <v>628</v>
       </c>
       <c r="C31" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D31">
         <v>50</v>
@@ -20993,7 +20987,7 @@
         <v>628</v>
       </c>
       <c r="C32" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D32">
         <v>50</v>
@@ -21007,7 +21001,7 @@
         <v>627</v>
       </c>
       <c r="C33" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D33">
         <v>50</v>
@@ -21021,7 +21015,7 @@
         <v>627</v>
       </c>
       <c r="C34" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D34">
         <v>50</v>
@@ -21035,7 +21029,7 @@
         <v>627</v>
       </c>
       <c r="C35" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D35">
         <v>50</v>
@@ -21049,7 +21043,7 @@
         <v>610</v>
       </c>
       <c r="C36" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D36">
         <v>50</v>
@@ -21063,7 +21057,7 @@
         <v>610</v>
       </c>
       <c r="C37" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D37">
         <v>50</v>
@@ -21077,7 +21071,7 @@
         <v>609</v>
       </c>
       <c r="C38" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D38">
         <v>50</v>
@@ -21091,7 +21085,7 @@
         <v>609</v>
       </c>
       <c r="C39" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D39">
         <v>50</v>
@@ -21119,7 +21113,7 @@
         <v>622</v>
       </c>
       <c r="C41" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D41">
         <v>50</v>
@@ -21133,7 +21127,7 @@
         <v>622</v>
       </c>
       <c r="C42" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D42">
         <v>50</v>
@@ -21161,7 +21155,7 @@
         <v>621</v>
       </c>
       <c r="C44" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D44">
         <v>50</v>
@@ -21175,7 +21169,7 @@
         <v>621</v>
       </c>
       <c r="C45" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D45">
         <v>50</v>
@@ -21203,7 +21197,7 @@
         <v>618</v>
       </c>
       <c r="C47" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D47">
         <v>50</v>
@@ -21217,7 +21211,7 @@
         <v>618</v>
       </c>
       <c r="C48" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D48">
         <v>50</v>
@@ -21245,7 +21239,7 @@
         <v>617</v>
       </c>
       <c r="C50" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D50">
         <v>50</v>
@@ -21259,7 +21253,7 @@
         <v>617</v>
       </c>
       <c r="C51" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D51">
         <v>50</v>
@@ -21273,7 +21267,7 @@
         <v>624</v>
       </c>
       <c r="C52" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D52">
         <v>50</v>
@@ -21287,7 +21281,7 @@
         <v>624</v>
       </c>
       <c r="C53" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D53">
         <v>50</v>
@@ -21301,7 +21295,7 @@
         <v>624</v>
       </c>
       <c r="C54" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D54">
         <v>50</v>
@@ -21315,7 +21309,7 @@
         <v>624</v>
       </c>
       <c r="C55" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D55">
         <v>50</v>
@@ -21329,7 +21323,7 @@
         <v>623</v>
       </c>
       <c r="C56" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D56">
         <v>50</v>
@@ -21343,7 +21337,7 @@
         <v>623</v>
       </c>
       <c r="C57" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D57">
         <v>50</v>
@@ -21357,7 +21351,7 @@
         <v>623</v>
       </c>
       <c r="C58" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D58">
         <v>50</v>
@@ -21371,7 +21365,7 @@
         <v>623</v>
       </c>
       <c r="C59" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D59">
         <v>50</v>
@@ -21385,7 +21379,7 @@
         <v>620</v>
       </c>
       <c r="C60" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D60">
         <v>50</v>
@@ -21399,7 +21393,7 @@
         <v>620</v>
       </c>
       <c r="C61" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D61">
         <v>50</v>
@@ -21413,7 +21407,7 @@
         <v>620</v>
       </c>
       <c r="C62" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D62">
         <v>50</v>
@@ -21427,7 +21421,7 @@
         <v>619</v>
       </c>
       <c r="C63" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D63">
         <v>50</v>
@@ -21441,7 +21435,7 @@
         <v>619</v>
       </c>
       <c r="C64" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D64">
         <v>50</v>
@@ -21455,7 +21449,7 @@
         <v>619</v>
       </c>
       <c r="C65" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D65">
         <v>50</v>
@@ -21469,7 +21463,7 @@
         <v>614</v>
       </c>
       <c r="C66" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D66">
         <v>50</v>
@@ -21483,7 +21477,7 @@
         <v>614</v>
       </c>
       <c r="C67" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D67">
         <v>50</v>
@@ -21497,7 +21491,7 @@
         <v>614</v>
       </c>
       <c r="C68" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D68">
         <v>50</v>
@@ -21511,7 +21505,7 @@
         <v>613</v>
       </c>
       <c r="C69" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D69">
         <v>50</v>
@@ -21525,7 +21519,7 @@
         <v>613</v>
       </c>
       <c r="C70" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D70">
         <v>50</v>
@@ -21539,7 +21533,7 @@
         <v>613</v>
       </c>
       <c r="C71" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D71">
         <v>50</v>
@@ -21553,7 +21547,7 @@
         <v>612</v>
       </c>
       <c r="C72" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D72">
         <v>50</v>
@@ -21567,7 +21561,7 @@
         <v>612</v>
       </c>
       <c r="C73" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D73">
         <v>50</v>
@@ -21581,7 +21575,7 @@
         <v>612</v>
       </c>
       <c r="C74" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D74">
         <v>50</v>
@@ -21595,7 +21589,7 @@
         <v>611</v>
       </c>
       <c r="C75" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D75">
         <v>50</v>
@@ -21609,7 +21603,7 @@
         <v>611</v>
       </c>
       <c r="C76" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D76">
         <v>50</v>
@@ -21623,7 +21617,7 @@
         <v>611</v>
       </c>
       <c r="C77" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D77">
         <v>50</v>
@@ -21637,7 +21631,7 @@
         <v>607</v>
       </c>
       <c r="C78" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D78">
         <v>50</v>
@@ -21651,7 +21645,7 @@
         <v>607</v>
       </c>
       <c r="C79" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D79">
         <v>50</v>
@@ -21665,7 +21659,7 @@
         <v>607</v>
       </c>
       <c r="C80" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D80">
         <v>50</v>
@@ -21679,7 +21673,7 @@
         <v>606</v>
       </c>
       <c r="C81" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D81">
         <v>50</v>
@@ -21693,7 +21687,7 @@
         <v>606</v>
       </c>
       <c r="C82" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D82">
         <v>50</v>
@@ -21707,7 +21701,7 @@
         <v>606</v>
       </c>
       <c r="C83" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D83">
         <v>50</v>
@@ -21721,7 +21715,7 @@
         <v>603</v>
       </c>
       <c r="C84" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D84">
         <v>50</v>
@@ -21735,7 +21729,7 @@
         <v>603</v>
       </c>
       <c r="C85" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D85">
         <v>50</v>
@@ -21749,7 +21743,7 @@
         <v>603</v>
       </c>
       <c r="C86" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D86">
         <v>50</v>
@@ -21763,7 +21757,7 @@
         <v>602</v>
       </c>
       <c r="C87" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D87">
         <v>50</v>
@@ -21777,7 +21771,7 @@
         <v>602</v>
       </c>
       <c r="C88" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D88">
         <v>50</v>
@@ -21791,7 +21785,7 @@
         <v>602</v>
       </c>
       <c r="C89" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D89">
         <v>50</v>
@@ -21805,7 +21799,7 @@
         <v>601</v>
       </c>
       <c r="C90" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D90">
         <v>50</v>
@@ -21819,7 +21813,7 @@
         <v>601</v>
       </c>
       <c r="C91" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D91">
         <v>50</v>
@@ -21833,7 +21827,7 @@
         <v>601</v>
       </c>
       <c r="C92" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D92">
         <v>50</v>
@@ -21847,7 +21841,7 @@
         <v>601</v>
       </c>
       <c r="C93" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D93">
         <v>50</v>
@@ -21861,7 +21855,7 @@
         <v>601</v>
       </c>
       <c r="C94" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D94">
         <v>50</v>
@@ -21875,7 +21869,7 @@
         <v>599</v>
       </c>
       <c r="C95" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D95">
         <v>50</v>
@@ -21889,7 +21883,7 @@
         <v>599</v>
       </c>
       <c r="C96" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D96">
         <v>50</v>
@@ -21903,7 +21897,7 @@
         <v>599</v>
       </c>
       <c r="C97" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D97">
         <v>50</v>
@@ -21917,7 +21911,7 @@
         <v>597</v>
       </c>
       <c r="C98" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D98">
         <v>50</v>
@@ -21931,7 +21925,7 @@
         <v>597</v>
       </c>
       <c r="C99" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D99">
         <v>50</v>
@@ -21945,7 +21939,7 @@
         <v>597</v>
       </c>
       <c r="C100" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D100">
         <v>50</v>
@@ -21959,7 +21953,7 @@
         <v>598</v>
       </c>
       <c r="C101" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D101">
         <v>50</v>
@@ -21973,7 +21967,7 @@
         <v>598</v>
       </c>
       <c r="C102" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D102">
         <v>50</v>
@@ -21987,7 +21981,7 @@
         <v>598</v>
       </c>
       <c r="C103" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D103">
         <v>50</v>
@@ -22001,7 +21995,7 @@
         <v>596</v>
       </c>
       <c r="C104" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D104">
         <v>50</v>
@@ -22015,7 +22009,7 @@
         <v>596</v>
       </c>
       <c r="C105" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D105">
         <v>50</v>
@@ -22029,7 +22023,7 @@
         <v>596</v>
       </c>
       <c r="C106" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D106">
         <v>50</v>
@@ -22043,7 +22037,7 @@
         <v>595</v>
       </c>
       <c r="C107" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D107">
         <v>50</v>
@@ -22057,7 +22051,7 @@
         <v>595</v>
       </c>
       <c r="C108" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D108">
         <v>50</v>
@@ -22071,7 +22065,7 @@
         <v>595</v>
       </c>
       <c r="C109" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D109">
         <v>50</v>
@@ -22085,7 +22079,7 @@
         <v>594</v>
       </c>
       <c r="C110" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D110">
         <v>50</v>
@@ -22099,7 +22093,7 @@
         <v>594</v>
       </c>
       <c r="C111" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D111">
         <v>50</v>
@@ -22113,7 +22107,7 @@
         <v>594</v>
       </c>
       <c r="C112" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D112">
         <v>50</v>
@@ -22127,7 +22121,7 @@
         <v>592</v>
       </c>
       <c r="C113" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D113">
         <v>50</v>
@@ -22141,7 +22135,7 @@
         <v>592</v>
       </c>
       <c r="C114" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D114">
         <v>50</v>
@@ -22155,7 +22149,7 @@
         <v>592</v>
       </c>
       <c r="C115" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D115">
         <v>50</v>
@@ -22169,7 +22163,7 @@
         <v>593</v>
       </c>
       <c r="C116" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D116">
         <v>50</v>
@@ -22183,7 +22177,7 @@
         <v>593</v>
       </c>
       <c r="C117" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D117">
         <v>50</v>
@@ -22197,7 +22191,7 @@
         <v>593</v>
       </c>
       <c r="C118" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D118">
         <v>50</v>
@@ -22211,7 +22205,7 @@
         <v>591</v>
       </c>
       <c r="C119" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D119">
         <v>50</v>
@@ -22225,7 +22219,7 @@
         <v>591</v>
       </c>
       <c r="C120" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D120">
         <v>50</v>
@@ -22239,7 +22233,7 @@
         <v>591</v>
       </c>
       <c r="C121" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D121">
         <v>50</v>
@@ -22253,7 +22247,7 @@
         <v>589</v>
       </c>
       <c r="C122" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D122">
         <v>50</v>
@@ -22267,7 +22261,7 @@
         <v>589</v>
       </c>
       <c r="C123" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D123">
         <v>50</v>
@@ -22281,7 +22275,7 @@
         <v>589</v>
       </c>
       <c r="C124" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D124">
         <v>50</v>
@@ -22295,7 +22289,7 @@
         <v>590</v>
       </c>
       <c r="C125" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D125">
         <v>50</v>
@@ -22309,7 +22303,7 @@
         <v>590</v>
       </c>
       <c r="C126" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D126">
         <v>50</v>
@@ -22323,7 +22317,7 @@
         <v>590</v>
       </c>
       <c r="C127" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D127">
         <v>50</v>
@@ -22337,7 +22331,7 @@
         <v>588</v>
       </c>
       <c r="C128" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D128">
         <v>50</v>
@@ -22351,7 +22345,7 @@
         <v>588</v>
       </c>
       <c r="C129" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D129">
         <v>50</v>
@@ -22365,7 +22359,7 @@
         <v>588</v>
       </c>
       <c r="C130" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D130">
         <v>50</v>
@@ -22379,7 +22373,7 @@
         <v>586</v>
       </c>
       <c r="C131" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D131">
         <v>50</v>
@@ -22393,7 +22387,7 @@
         <v>586</v>
       </c>
       <c r="C132" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D132">
         <v>50</v>
@@ -22407,7 +22401,7 @@
         <v>586</v>
       </c>
       <c r="C133" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D133">
         <v>50</v>
@@ -22421,7 +22415,7 @@
         <v>587</v>
       </c>
       <c r="C134" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D134">
         <v>50</v>
@@ -22435,7 +22429,7 @@
         <v>587</v>
       </c>
       <c r="C135" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D135">
         <v>50</v>
@@ -22449,7 +22443,7 @@
         <v>587</v>
       </c>
       <c r="C136" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D136">
         <v>50</v>
@@ -22463,7 +22457,7 @@
         <v>582</v>
       </c>
       <c r="C137" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D137">
         <v>50</v>
@@ -22477,7 +22471,7 @@
         <v>582</v>
       </c>
       <c r="C138" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D138">
         <v>50</v>
@@ -22491,7 +22485,7 @@
         <v>581</v>
       </c>
       <c r="C139" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D139">
         <v>50</v>
@@ -22505,7 +22499,7 @@
         <v>581</v>
       </c>
       <c r="C140" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D140">
         <v>50</v>
@@ -22519,7 +22513,7 @@
         <v>482</v>
       </c>
       <c r="C141" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D141">
         <v>50</v>
@@ -22533,7 +22527,7 @@
         <v>482</v>
       </c>
       <c r="C142" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D142">
         <v>50</v>
@@ -22547,7 +22541,7 @@
         <v>494</v>
       </c>
       <c r="C143" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D143">
         <v>50</v>
@@ -22561,7 +22555,7 @@
         <v>494</v>
       </c>
       <c r="C144" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D144">
         <v>50</v>
@@ -22575,7 +22569,7 @@
         <v>574</v>
       </c>
       <c r="C145" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D145">
         <v>50</v>
@@ -22589,7 +22583,7 @@
         <v>573</v>
       </c>
       <c r="C146" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D146">
         <v>50</v>
@@ -22603,7 +22597,7 @@
         <v>573</v>
       </c>
       <c r="C147" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D147">
         <v>50</v>
@@ -22617,7 +22611,7 @@
         <v>572</v>
       </c>
       <c r="C148" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D148">
         <v>50</v>
@@ -22631,7 +22625,7 @@
         <v>572</v>
       </c>
       <c r="C149" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D149">
         <v>50</v>
@@ -22645,7 +22639,7 @@
         <v>578</v>
       </c>
       <c r="C150" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D150">
         <v>50</v>
@@ -22659,7 +22653,7 @@
         <v>578</v>
       </c>
       <c r="C151" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D151">
         <v>50</v>
@@ -22673,7 +22667,7 @@
         <v>578</v>
       </c>
       <c r="C152" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D152">
         <v>50</v>
@@ -22687,7 +22681,7 @@
         <v>569</v>
       </c>
       <c r="C153" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D153">
         <v>50</v>
@@ -22701,7 +22695,7 @@
         <v>569</v>
       </c>
       <c r="C154" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D154">
         <v>50</v>
@@ -22715,7 +22709,7 @@
         <v>567</v>
       </c>
       <c r="C155" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D155">
         <v>50</v>
@@ -22729,7 +22723,7 @@
         <v>567</v>
       </c>
       <c r="C156" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D156">
         <v>50</v>
@@ -22743,7 +22737,7 @@
         <v>566</v>
       </c>
       <c r="C157" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D157">
         <v>50</v>
@@ -22757,7 +22751,7 @@
         <v>566</v>
       </c>
       <c r="C158" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D158">
         <v>50</v>
@@ -22771,7 +22765,7 @@
         <v>563</v>
       </c>
       <c r="C159" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D159">
         <v>50</v>
@@ -22785,7 +22779,7 @@
         <v>563</v>
       </c>
       <c r="C160" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D160">
         <v>50</v>
@@ -22799,7 +22793,7 @@
         <v>561</v>
       </c>
       <c r="C161" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D161">
         <v>50</v>
@@ -22813,7 +22807,7 @@
         <v>561</v>
       </c>
       <c r="C162" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D162">
         <v>50</v>
@@ -22827,7 +22821,7 @@
         <v>559</v>
       </c>
       <c r="C163" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D163">
         <v>50</v>
@@ -22841,7 +22835,7 @@
         <v>559</v>
       </c>
       <c r="C164" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D164">
         <v>50</v>
@@ -22855,7 +22849,7 @@
         <v>559</v>
       </c>
       <c r="C165" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D165">
         <v>50</v>
@@ -22869,7 +22863,7 @@
         <v>557</v>
       </c>
       <c r="C166" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D166">
         <v>50</v>
@@ -22883,7 +22877,7 @@
         <v>557</v>
       </c>
       <c r="C167" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D167">
         <v>50</v>
@@ -22897,7 +22891,7 @@
         <v>557</v>
       </c>
       <c r="C168" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D168">
         <v>50</v>
@@ -22911,7 +22905,7 @@
         <v>558</v>
       </c>
       <c r="C169" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D169">
         <v>50</v>
@@ -22925,7 +22919,7 @@
         <v>558</v>
       </c>
       <c r="C170" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D170">
         <v>50</v>
@@ -22939,7 +22933,7 @@
         <v>558</v>
       </c>
       <c r="C171" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D171">
         <v>50</v>
@@ -22953,7 +22947,7 @@
         <v>556</v>
       </c>
       <c r="C172" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D172">
         <v>50</v>
@@ -22967,7 +22961,7 @@
         <v>556</v>
       </c>
       <c r="C173" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D173">
         <v>50</v>
@@ -22981,7 +22975,7 @@
         <v>556</v>
       </c>
       <c r="C174" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D174">
         <v>50</v>
@@ -22995,7 +22989,7 @@
         <v>555</v>
       </c>
       <c r="C175" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D175">
         <v>50</v>
@@ -23009,7 +23003,7 @@
         <v>555</v>
       </c>
       <c r="C176" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D176">
         <v>50</v>
@@ -23023,7 +23017,7 @@
         <v>555</v>
       </c>
       <c r="C177" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D177">
         <v>50</v>
@@ -23037,7 +23031,7 @@
         <v>553</v>
       </c>
       <c r="C178" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D178">
         <v>50</v>
@@ -23051,7 +23045,7 @@
         <v>553</v>
       </c>
       <c r="C179" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D179">
         <v>50</v>
@@ -23065,7 +23059,7 @@
         <v>553</v>
       </c>
       <c r="C180" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D180">
         <v>50</v>
@@ -23079,7 +23073,7 @@
         <v>551</v>
       </c>
       <c r="C181" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D181">
         <v>50</v>
@@ -23093,7 +23087,7 @@
         <v>551</v>
       </c>
       <c r="C182" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D182">
         <v>50</v>
@@ -23107,7 +23101,7 @@
         <v>551</v>
       </c>
       <c r="C183" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D183">
         <v>50</v>
@@ -23121,7 +23115,7 @@
         <v>550</v>
       </c>
       <c r="C184" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D184">
         <v>50</v>
@@ -23135,7 +23129,7 @@
         <v>550</v>
       </c>
       <c r="C185" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D185">
         <v>50</v>
@@ -23149,7 +23143,7 @@
         <v>550</v>
       </c>
       <c r="C186" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D186">
         <v>50</v>
@@ -23163,7 +23157,7 @@
         <v>549</v>
       </c>
       <c r="C187" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D187">
         <v>50</v>
@@ -23177,7 +23171,7 @@
         <v>549</v>
       </c>
       <c r="C188" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D188">
         <v>50</v>
@@ -23191,7 +23185,7 @@
         <v>547</v>
       </c>
       <c r="C189" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D189">
         <v>50</v>
@@ -23205,7 +23199,7 @@
         <v>547</v>
       </c>
       <c r="C190" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D190">
         <v>50</v>
@@ -23219,7 +23213,7 @@
         <v>546</v>
       </c>
       <c r="C191" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D191">
         <v>50</v>
@@ -23233,7 +23227,7 @@
         <v>545</v>
       </c>
       <c r="C192" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D192">
         <v>50</v>
@@ -23247,7 +23241,7 @@
         <v>545</v>
       </c>
       <c r="C193" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D193">
         <v>50</v>
@@ -23261,7 +23255,7 @@
         <v>543</v>
       </c>
       <c r="C194" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D194">
         <v>50</v>
@@ -23275,7 +23269,7 @@
         <v>543</v>
       </c>
       <c r="C195" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D195">
         <v>50</v>
@@ -23289,7 +23283,7 @@
         <v>541</v>
       </c>
       <c r="C196" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D196">
         <v>50</v>
@@ -23303,7 +23297,7 @@
         <v>541</v>
       </c>
       <c r="C197" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D197">
         <v>50</v>
@@ -23317,7 +23311,7 @@
         <v>541</v>
       </c>
       <c r="C198" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D198">
         <v>50</v>
@@ -23331,7 +23325,7 @@
         <v>540</v>
       </c>
       <c r="C199" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D199">
         <v>50</v>
@@ -23345,7 +23339,7 @@
         <v>540</v>
       </c>
       <c r="C200" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D200">
         <v>50</v>
@@ -23359,7 +23353,7 @@
         <v>540</v>
       </c>
       <c r="C201" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D201">
         <v>50</v>
@@ -23373,7 +23367,7 @@
         <v>537</v>
       </c>
       <c r="C202" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D202">
         <v>50</v>
@@ -23387,7 +23381,7 @@
         <v>537</v>
       </c>
       <c r="C203" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D203">
         <v>50</v>
@@ -23401,7 +23395,7 @@
         <v>537</v>
       </c>
       <c r="C204" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D204">
         <v>50</v>
@@ -23415,7 +23409,7 @@
         <v>536</v>
       </c>
       <c r="C205" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D205">
         <v>50</v>
@@ -23429,7 +23423,7 @@
         <v>536</v>
       </c>
       <c r="C206" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D206">
         <v>50</v>
@@ -23443,7 +23437,7 @@
         <v>536</v>
       </c>
       <c r="C207" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D207">
         <v>50</v>
@@ -23457,7 +23451,7 @@
         <v>535</v>
       </c>
       <c r="C208" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D208">
         <v>50</v>
@@ -23471,7 +23465,7 @@
         <v>535</v>
       </c>
       <c r="C209" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D209">
         <v>50</v>
@@ -23485,7 +23479,7 @@
         <v>535</v>
       </c>
       <c r="C210" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D210">
         <v>50</v>
@@ -23499,7 +23493,7 @@
         <v>533</v>
       </c>
       <c r="C211" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D211">
         <v>50</v>
@@ -23513,7 +23507,7 @@
         <v>533</v>
       </c>
       <c r="C212" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D212">
         <v>50</v>
@@ -23527,7 +23521,7 @@
         <v>533</v>
       </c>
       <c r="C213" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D213">
         <v>50</v>
@@ -23541,7 +23535,7 @@
         <v>533</v>
       </c>
       <c r="C214" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D214">
         <v>50</v>
@@ -23555,7 +23549,7 @@
         <v>532</v>
       </c>
       <c r="C215" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D215">
         <v>50</v>
@@ -23569,7 +23563,7 @@
         <v>532</v>
       </c>
       <c r="C216" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D216">
         <v>50</v>
@@ -23583,7 +23577,7 @@
         <v>532</v>
       </c>
       <c r="C217" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D217">
         <v>50</v>
@@ -23597,7 +23591,7 @@
         <v>532</v>
       </c>
       <c r="C218" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D218">
         <v>50</v>
@@ -23611,7 +23605,7 @@
         <v>531</v>
       </c>
       <c r="C219" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D219">
         <v>50</v>
@@ -23625,7 +23619,7 @@
         <v>531</v>
       </c>
       <c r="C220" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D220">
         <v>50</v>
@@ -23639,7 +23633,7 @@
         <v>531</v>
       </c>
       <c r="C221" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D221">
         <v>50</v>
@@ -23653,7 +23647,7 @@
         <v>530</v>
       </c>
       <c r="C222" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D222">
         <v>50</v>
@@ -23667,7 +23661,7 @@
         <v>530</v>
       </c>
       <c r="C223" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D223">
         <v>50</v>
@@ -23681,7 +23675,7 @@
         <v>530</v>
       </c>
       <c r="C224" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D224">
         <v>50</v>
@@ -23695,7 +23689,7 @@
         <v>529</v>
       </c>
       <c r="C225" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D225">
         <v>50</v>
@@ -23709,7 +23703,7 @@
         <v>529</v>
       </c>
       <c r="C226" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D226">
         <v>50</v>
@@ -23723,7 +23717,7 @@
         <v>529</v>
       </c>
       <c r="C227" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D227">
         <v>50</v>
@@ -23737,7 +23731,7 @@
         <v>527</v>
       </c>
       <c r="C228" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D228">
         <v>50</v>
@@ -23751,7 +23745,7 @@
         <v>527</v>
       </c>
       <c r="C229" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D229">
         <v>50</v>
@@ -23765,7 +23759,7 @@
         <v>527</v>
       </c>
       <c r="C230" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D230">
         <v>50</v>
@@ -23779,7 +23773,7 @@
         <v>528</v>
       </c>
       <c r="C231" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D231">
         <v>50</v>
@@ -23793,7 +23787,7 @@
         <v>528</v>
       </c>
       <c r="C232" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D232">
         <v>50</v>
@@ -23807,7 +23801,7 @@
         <v>528</v>
       </c>
       <c r="C233" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D233">
         <v>50</v>
@@ -23821,7 +23815,7 @@
         <v>526</v>
       </c>
       <c r="C234" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D234">
         <v>50</v>
@@ -23835,7 +23829,7 @@
         <v>526</v>
       </c>
       <c r="C235" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D235">
         <v>50</v>
@@ -23849,7 +23843,7 @@
         <v>526</v>
       </c>
       <c r="C236" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D236">
         <v>50</v>
@@ -23863,7 +23857,7 @@
         <v>525</v>
       </c>
       <c r="C237" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D237">
         <v>50</v>
@@ -23877,7 +23871,7 @@
         <v>525</v>
       </c>
       <c r="C238" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D238">
         <v>50</v>
@@ -23891,7 +23885,7 @@
         <v>525</v>
       </c>
       <c r="C239" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D239">
         <v>50</v>
@@ -23905,7 +23899,7 @@
         <v>512</v>
       </c>
       <c r="C240" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D240">
         <v>50</v>
@@ -23919,7 +23913,7 @@
         <v>493</v>
       </c>
       <c r="C241" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D241">
         <v>50</v>
@@ -23933,7 +23927,7 @@
         <v>493</v>
       </c>
       <c r="C242" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D242">
         <v>50</v>
@@ -23947,7 +23941,7 @@
         <v>493</v>
       </c>
       <c r="C243" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D243">
         <v>50</v>
@@ -23961,7 +23955,7 @@
         <v>473</v>
       </c>
       <c r="C244" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D244">
         <v>50</v>
@@ -23975,7 +23969,7 @@
         <v>473</v>
       </c>
       <c r="C245" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D245">
         <v>50</v>
@@ -23989,7 +23983,7 @@
         <v>473</v>
       </c>
       <c r="C246" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D246">
         <v>50</v>
@@ -24003,7 +23997,7 @@
         <v>472</v>
       </c>
       <c r="C247" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D247">
         <v>50</v>
@@ -24017,7 +24011,7 @@
         <v>472</v>
       </c>
       <c r="C248" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D248">
         <v>50</v>
@@ -24031,7 +24025,7 @@
         <v>472</v>
       </c>
       <c r="C249" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D249">
         <v>50</v>
@@ -24045,7 +24039,7 @@
         <v>501</v>
       </c>
       <c r="C250" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D250">
         <v>50</v>
@@ -24059,7 +24053,7 @@
         <v>495</v>
       </c>
       <c r="C251" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D251">
         <v>50</v>
@@ -24073,7 +24067,7 @@
         <v>496</v>
       </c>
       <c r="C252" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D252">
         <v>50</v>
@@ -24087,7 +24081,7 @@
         <v>497</v>
       </c>
       <c r="C253" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D253">
         <v>50</v>
@@ -24101,7 +24095,7 @@
         <v>498</v>
       </c>
       <c r="C254" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D254">
         <v>50</v>
@@ -24115,7 +24109,7 @@
         <v>499</v>
       </c>
       <c r="C255" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D255">
         <v>50</v>
@@ -24129,7 +24123,7 @@
         <v>500</v>
       </c>
       <c r="C256" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D256">
         <v>50</v>
@@ -24143,7 +24137,7 @@
         <v>469</v>
       </c>
       <c r="C257" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D257">
         <v>50</v>
@@ -24157,7 +24151,7 @@
         <v>469</v>
       </c>
       <c r="C258" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D258">
         <v>50</v>
@@ -24171,7 +24165,7 @@
         <v>506</v>
       </c>
       <c r="C259" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D259">
         <v>50</v>
@@ -24185,7 +24179,7 @@
         <v>506</v>
       </c>
       <c r="C260" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D260">
         <v>50</v>
@@ -24199,7 +24193,7 @@
         <v>452</v>
       </c>
       <c r="C261" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D261">
         <v>50</v>
@@ -24213,7 +24207,7 @@
         <v>452</v>
       </c>
       <c r="C262" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D262">
         <v>50</v>
@@ -24227,7 +24221,7 @@
         <v>517</v>
       </c>
       <c r="C263" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D263">
         <v>50</v>
@@ -24241,7 +24235,7 @@
         <v>517</v>
       </c>
       <c r="C264" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D264">
         <v>50</v>
@@ -24255,7 +24249,7 @@
         <v>461</v>
       </c>
       <c r="C265" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D265">
         <v>50</v>
@@ -24269,7 +24263,7 @@
         <v>461</v>
       </c>
       <c r="C266" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D266">
         <v>50</v>
@@ -24283,7 +24277,7 @@
         <v>508</v>
       </c>
       <c r="C267" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D267">
         <v>50</v>
@@ -24297,7 +24291,7 @@
         <v>508</v>
       </c>
       <c r="C268" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D268">
         <v>50</v>
@@ -24311,7 +24305,7 @@
         <v>470</v>
       </c>
       <c r="C269" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D269">
         <v>50</v>
@@ -24325,7 +24319,7 @@
         <v>470</v>
       </c>
       <c r="C270" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D270">
         <v>50</v>
@@ -24339,7 +24333,7 @@
         <v>484</v>
       </c>
       <c r="C271" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D271">
         <v>50</v>
@@ -24353,7 +24347,7 @@
         <v>484</v>
       </c>
       <c r="C272" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D272">
         <v>50</v>
@@ -24367,7 +24361,7 @@
         <v>484</v>
       </c>
       <c r="C273" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D273">
         <v>50</v>
@@ -24381,7 +24375,7 @@
         <v>476</v>
       </c>
       <c r="C274" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D274">
         <v>50</v>
@@ -24395,7 +24389,7 @@
         <v>476</v>
       </c>
       <c r="C275" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D275">
         <v>50</v>
@@ -24409,7 +24403,7 @@
         <v>462</v>
       </c>
       <c r="C276" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D276">
         <v>50</v>
@@ -24423,7 +24417,7 @@
         <v>462</v>
       </c>
       <c r="C277" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D277">
         <v>50</v>
@@ -24437,7 +24431,7 @@
         <v>463</v>
       </c>
       <c r="C278" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D278">
         <v>50</v>
@@ -24451,7 +24445,7 @@
         <v>463</v>
       </c>
       <c r="C279" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D279">
         <v>50</v>
@@ -24465,7 +24459,7 @@
         <v>455</v>
       </c>
       <c r="C280" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D280">
         <v>50</v>
@@ -24479,7 +24473,7 @@
         <v>455</v>
       </c>
       <c r="C281" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D281">
         <v>50</v>
@@ -24493,7 +24487,7 @@
         <v>456</v>
       </c>
       <c r="C282" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D282">
         <v>50</v>
@@ -24507,7 +24501,7 @@
         <v>456</v>
       </c>
       <c r="C283" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D283">
         <v>50</v>
@@ -24521,7 +24515,7 @@
         <v>218</v>
       </c>
       <c r="C284" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D284">
         <v>50</v>
@@ -24535,7 +24529,7 @@
         <v>218</v>
       </c>
       <c r="C285" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D285">
         <v>50</v>
@@ -24549,7 +24543,7 @@
         <v>460</v>
       </c>
       <c r="C286" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D286">
         <v>50</v>
@@ -24563,7 +24557,7 @@
         <v>460</v>
       </c>
       <c r="C287" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D287">
         <v>50</v>
@@ -24577,7 +24571,7 @@
         <v>445</v>
       </c>
       <c r="C288" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D288">
         <v>50</v>
@@ -24591,7 +24585,7 @@
         <v>445</v>
       </c>
       <c r="C289" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D289">
         <v>50</v>
@@ -24605,7 +24599,7 @@
         <v>404</v>
       </c>
       <c r="C290" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D290">
         <v>50</v>
@@ -24619,7 +24613,7 @@
         <v>404</v>
       </c>
       <c r="C291" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D291">
         <v>50</v>
@@ -24633,7 +24627,7 @@
         <v>404</v>
       </c>
       <c r="C292" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D292">
         <v>50</v>
@@ -24647,7 +24641,7 @@
         <v>403</v>
       </c>
       <c r="C293" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D293">
         <v>50</v>
@@ -24661,7 +24655,7 @@
         <v>403</v>
       </c>
       <c r="C294" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D294">
         <v>50</v>
@@ -24675,7 +24669,7 @@
         <v>403</v>
       </c>
       <c r="C295" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D295">
         <v>50</v>
@@ -24689,7 +24683,7 @@
         <v>405</v>
       </c>
       <c r="C296" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D296">
         <v>50</v>
@@ -24703,7 +24697,7 @@
         <v>451</v>
       </c>
       <c r="C297" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D297">
         <v>50</v>
@@ -24717,7 +24711,7 @@
         <v>451</v>
       </c>
       <c r="C298" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D298">
         <v>50</v>
@@ -24731,7 +24725,7 @@
         <v>451</v>
       </c>
       <c r="C299" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D299">
         <v>50</v>
@@ -24745,7 +24739,7 @@
         <v>449</v>
       </c>
       <c r="C300" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D300">
         <v>50</v>
@@ -24759,7 +24753,7 @@
         <v>449</v>
       </c>
       <c r="C301" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D301">
         <v>50</v>
@@ -24773,7 +24767,7 @@
         <v>449</v>
       </c>
       <c r="C302" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D302">
         <v>50</v>
@@ -24787,7 +24781,7 @@
         <v>450</v>
       </c>
       <c r="C303" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D303">
         <v>50</v>
@@ -24801,7 +24795,7 @@
         <v>450</v>
       </c>
       <c r="C304" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D304">
         <v>50</v>
@@ -24815,7 +24809,7 @@
         <v>450</v>
       </c>
       <c r="C305" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D305">
         <v>50</v>
@@ -24829,7 +24823,7 @@
         <v>468</v>
       </c>
       <c r="C306" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D306">
         <v>50</v>
@@ -24843,7 +24837,7 @@
         <v>468</v>
       </c>
       <c r="C307" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D307">
         <v>50</v>
@@ -24857,7 +24851,7 @@
         <v>468</v>
       </c>
       <c r="C308" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D308">
         <v>50</v>
@@ -24871,7 +24865,7 @@
         <v>319</v>
       </c>
       <c r="C309" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D309">
         <v>50</v>
@@ -24885,7 +24879,7 @@
         <v>319</v>
       </c>
       <c r="C310" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D310">
         <v>50</v>
@@ -24899,7 +24893,7 @@
         <v>319</v>
       </c>
       <c r="C311" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D311">
         <v>50</v>
@@ -24913,7 +24907,7 @@
         <v>321</v>
       </c>
       <c r="C312" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D312">
         <v>50</v>
@@ -24927,7 +24921,7 @@
         <v>321</v>
       </c>
       <c r="C313" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D313">
         <v>50</v>
@@ -24941,7 +24935,7 @@
         <v>321</v>
       </c>
       <c r="C314" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D314">
         <v>50</v>
@@ -24955,7 +24949,7 @@
         <v>364</v>
       </c>
       <c r="C315" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D315">
         <v>50</v>
@@ -24969,7 +24963,7 @@
         <v>364</v>
       </c>
       <c r="C316" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D316">
         <v>50</v>
@@ -24983,7 +24977,7 @@
         <v>364</v>
       </c>
       <c r="C317" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D317">
         <v>50</v>
@@ -24997,7 +24991,7 @@
         <v>338</v>
       </c>
       <c r="C318" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D318">
         <v>50</v>
@@ -25011,7 +25005,7 @@
         <v>338</v>
       </c>
       <c r="C319" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D319">
         <v>50</v>
@@ -25025,7 +25019,7 @@
         <v>338</v>
       </c>
       <c r="C320" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D320">
         <v>50</v>
@@ -25039,7 +25033,7 @@
         <v>338</v>
       </c>
       <c r="C321" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D321">
         <v>50</v>
@@ -25053,7 +25047,7 @@
         <v>93</v>
       </c>
       <c r="C322" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D322">
         <v>50</v>
@@ -25067,7 +25061,7 @@
         <v>93</v>
       </c>
       <c r="C323" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D323">
         <v>50</v>
@@ -25081,7 +25075,7 @@
         <v>93</v>
       </c>
       <c r="C324" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D324">
         <v>50</v>
@@ -25095,7 +25089,7 @@
         <v>93</v>
       </c>
       <c r="C325" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D325">
         <v>50</v>
@@ -25109,7 +25103,7 @@
         <v>95</v>
       </c>
       <c r="C326" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D326">
         <v>50</v>
@@ -25123,7 +25117,7 @@
         <v>95</v>
       </c>
       <c r="C327" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D327">
         <v>50</v>
@@ -25137,7 +25131,7 @@
         <v>95</v>
       </c>
       <c r="C328" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D328">
         <v>50</v>
@@ -25151,7 +25145,7 @@
         <v>95</v>
       </c>
       <c r="C329" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D329">
         <v>50</v>
@@ -25165,7 +25159,7 @@
         <v>73</v>
       </c>
       <c r="C330" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D330">
         <v>50</v>
@@ -25179,7 +25173,7 @@
         <v>73</v>
       </c>
       <c r="C331" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D331">
         <v>50</v>
@@ -25193,7 +25187,7 @@
         <v>73</v>
       </c>
       <c r="C332" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D332">
         <v>50</v>
@@ -25207,7 +25201,7 @@
         <v>73</v>
       </c>
       <c r="C333" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D333">
         <v>50</v>
@@ -25221,7 +25215,7 @@
         <v>71</v>
       </c>
       <c r="C334" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D334">
         <v>50</v>
@@ -25235,7 +25229,7 @@
         <v>71</v>
       </c>
       <c r="C335" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D335">
         <v>50</v>
@@ -25249,7 +25243,7 @@
         <v>71</v>
       </c>
       <c r="C336" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D336">
         <v>50</v>
@@ -25263,7 +25257,7 @@
         <v>71</v>
       </c>
       <c r="C337" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D337">
         <v>50</v>
@@ -25277,7 +25271,7 @@
         <v>72</v>
       </c>
       <c r="C338" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D338">
         <v>50</v>
@@ -25291,7 +25285,7 @@
         <v>72</v>
       </c>
       <c r="C339" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D339">
         <v>50</v>
@@ -25305,7 +25299,7 @@
         <v>72</v>
       </c>
       <c r="C340" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D340">
         <v>50</v>
@@ -25319,7 +25313,7 @@
         <v>72</v>
       </c>
       <c r="C341" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D341">
         <v>50</v>
@@ -25333,7 +25327,7 @@
         <v>480</v>
       </c>
       <c r="C342" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D342">
         <v>50</v>
@@ -25347,7 +25341,7 @@
         <v>480</v>
       </c>
       <c r="C343" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D343">
         <v>50</v>
@@ -25361,7 +25355,7 @@
         <v>480</v>
       </c>
       <c r="C344" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D344">
         <v>50</v>
@@ -25375,7 +25369,7 @@
         <v>480</v>
       </c>
       <c r="C345" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D345">
         <v>50</v>
@@ -25389,7 +25383,7 @@
         <v>325</v>
       </c>
       <c r="C346" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D346">
         <v>50</v>
@@ -25403,7 +25397,7 @@
         <v>325</v>
       </c>
       <c r="C347" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D347">
         <v>50</v>
@@ -25417,7 +25411,7 @@
         <v>325</v>
       </c>
       <c r="C348" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D348">
         <v>50</v>
@@ -25431,7 +25425,7 @@
         <v>325</v>
       </c>
       <c r="C349" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D349">
         <v>50</v>
@@ -25445,7 +25439,7 @@
         <v>256</v>
       </c>
       <c r="C350" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D350">
         <v>50</v>
@@ -25459,7 +25453,7 @@
         <v>256</v>
       </c>
       <c r="C351" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D351">
         <v>50</v>
@@ -25473,7 +25467,7 @@
         <v>256</v>
       </c>
       <c r="C352" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D352">
         <v>50</v>
@@ -25487,7 +25481,7 @@
         <v>256</v>
       </c>
       <c r="C353" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D353">
         <v>50</v>
@@ -25501,7 +25495,7 @@
         <v>257</v>
       </c>
       <c r="C354" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D354">
         <v>50</v>
@@ -25515,7 +25509,7 @@
         <v>257</v>
       </c>
       <c r="C355" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D355">
         <v>50</v>
@@ -25529,7 +25523,7 @@
         <v>257</v>
       </c>
       <c r="C356" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D356">
         <v>50</v>
@@ -25543,7 +25537,7 @@
         <v>257</v>
       </c>
       <c r="C357" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D357">
         <v>50</v>
@@ -25557,7 +25551,7 @@
         <v>327</v>
       </c>
       <c r="C358" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D358">
         <v>50</v>
@@ -25571,7 +25565,7 @@
         <v>327</v>
       </c>
       <c r="C359" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D359">
         <v>50</v>
@@ -25585,7 +25579,7 @@
         <v>327</v>
       </c>
       <c r="C360" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D360">
         <v>50</v>
@@ -25599,7 +25593,7 @@
         <v>327</v>
       </c>
       <c r="C361" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D361">
         <v>50</v>
@@ -25613,7 +25607,7 @@
         <v>326</v>
       </c>
       <c r="C362" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D362">
         <v>50</v>
@@ -25627,7 +25621,7 @@
         <v>326</v>
       </c>
       <c r="C363" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D363">
         <v>50</v>
@@ -25641,7 +25635,7 @@
         <v>326</v>
       </c>
       <c r="C364" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D364">
         <v>50</v>
@@ -25655,7 +25649,7 @@
         <v>326</v>
       </c>
       <c r="C365" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D365">
         <v>50</v>
@@ -25669,7 +25663,7 @@
         <v>310</v>
       </c>
       <c r="C366" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D366">
         <v>50</v>
@@ -25683,7 +25677,7 @@
         <v>278</v>
       </c>
       <c r="C367" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D367">
         <v>50</v>
@@ -25697,7 +25691,7 @@
         <v>322</v>
       </c>
       <c r="C368" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D368">
         <v>50</v>
@@ -25711,7 +25705,7 @@
         <v>311</v>
       </c>
       <c r="C369" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D369">
         <v>50</v>
@@ -25725,7 +25719,7 @@
         <v>299</v>
       </c>
       <c r="C370" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D370">
         <v>50</v>
@@ -25739,7 +25733,7 @@
         <v>299</v>
       </c>
       <c r="C371" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D371">
         <v>50</v>
@@ -25753,7 +25747,7 @@
         <v>299</v>
       </c>
       <c r="C372" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D372">
         <v>50</v>
@@ -25767,7 +25761,7 @@
         <v>299</v>
       </c>
       <c r="C373" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D373">
         <v>50</v>
@@ -25781,7 +25775,7 @@
         <v>274</v>
       </c>
       <c r="C374" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D374">
         <v>50</v>
@@ -25795,7 +25789,7 @@
         <v>274</v>
       </c>
       <c r="C375" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D375">
         <v>50</v>
@@ -25809,7 +25803,7 @@
         <v>274</v>
       </c>
       <c r="C376" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D376">
         <v>50</v>
@@ -25823,7 +25817,7 @@
         <v>274</v>
       </c>
       <c r="C377" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D377">
         <v>50</v>
@@ -25837,7 +25831,7 @@
         <v>272</v>
       </c>
       <c r="C378" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D378">
         <v>50</v>
@@ -25851,7 +25845,7 @@
         <v>272</v>
       </c>
       <c r="C379" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D379">
         <v>50</v>
@@ -25865,7 +25859,7 @@
         <v>272</v>
       </c>
       <c r="C380" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D380">
         <v>50</v>
@@ -25879,7 +25873,7 @@
         <v>272</v>
       </c>
       <c r="C381" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D381">
         <v>50</v>
@@ -25893,7 +25887,7 @@
         <v>273</v>
       </c>
       <c r="C382" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D382">
         <v>50</v>
@@ -25907,7 +25901,7 @@
         <v>273</v>
       </c>
       <c r="C383" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D383">
         <v>50</v>
@@ -25921,7 +25915,7 @@
         <v>273</v>
       </c>
       <c r="C384" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D384">
         <v>50</v>
@@ -25935,7 +25929,7 @@
         <v>273</v>
       </c>
       <c r="C385" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D385">
         <v>50</v>
@@ -25949,7 +25943,7 @@
         <v>229</v>
       </c>
       <c r="C386" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D386">
         <v>50</v>
@@ -25963,7 +25957,7 @@
         <v>229</v>
       </c>
       <c r="C387" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D387">
         <v>50</v>
@@ -25977,7 +25971,7 @@
         <v>229</v>
       </c>
       <c r="C388" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D388">
         <v>50</v>
@@ -25991,7 +25985,7 @@
         <v>229</v>
       </c>
       <c r="C389" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D389">
         <v>50</v>
@@ -26005,7 +25999,7 @@
         <v>160</v>
       </c>
       <c r="C390" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D390">
         <v>50</v>
@@ -26019,7 +26013,7 @@
         <v>159</v>
       </c>
       <c r="C391" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D391">
         <v>50</v>
@@ -26033,7 +26027,7 @@
         <v>158</v>
       </c>
       <c r="C392" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D392">
         <v>50</v>
@@ -26047,7 +26041,7 @@
         <v>157</v>
       </c>
       <c r="C393" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D393">
         <v>50</v>
@@ -26061,7 +26055,7 @@
         <v>298</v>
       </c>
       <c r="C394" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D394">
         <v>50</v>
@@ -26075,7 +26069,7 @@
         <v>302</v>
       </c>
       <c r="C395" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D395">
         <v>50</v>
@@ -26089,7 +26083,7 @@
         <v>302</v>
       </c>
       <c r="C396" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D396">
         <v>50</v>
@@ -26103,7 +26097,7 @@
         <v>302</v>
       </c>
       <c r="C397" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D397">
         <v>50</v>
@@ -26117,7 +26111,7 @@
         <v>302</v>
       </c>
       <c r="C398" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D398">
         <v>50</v>
@@ -26131,7 +26125,7 @@
         <v>101</v>
       </c>
       <c r="C399" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D399">
         <v>50</v>
@@ -26145,7 +26139,7 @@
         <v>101</v>
       </c>
       <c r="C400" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D400">
         <v>50</v>
@@ -26159,7 +26153,7 @@
         <v>101</v>
       </c>
       <c r="C401" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D401">
         <v>50</v>
@@ -26173,7 +26167,7 @@
         <v>101</v>
       </c>
       <c r="C402" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D402">
         <v>50</v>
@@ -26187,7 +26181,7 @@
         <v>102</v>
       </c>
       <c r="C403" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D403">
         <v>50</v>
@@ -26201,7 +26195,7 @@
         <v>102</v>
       </c>
       <c r="C404" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D404">
         <v>50</v>
@@ -26215,7 +26209,7 @@
         <v>102</v>
       </c>
       <c r="C405" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D405">
         <v>50</v>
@@ -26229,7 +26223,7 @@
         <v>102</v>
       </c>
       <c r="C406" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D406">
         <v>50</v>
@@ -26243,7 +26237,7 @@
         <v>474</v>
       </c>
       <c r="C407" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D407">
         <v>50</v>
@@ -26257,7 +26251,7 @@
         <v>474</v>
       </c>
       <c r="C408" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D408">
         <v>50</v>
@@ -26271,7 +26265,7 @@
         <v>474</v>
       </c>
       <c r="C409" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D409">
         <v>50</v>
@@ -26285,7 +26279,7 @@
         <v>474</v>
       </c>
       <c r="C410" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D410">
         <v>50</v>
@@ -26299,7 +26293,7 @@
         <v>90</v>
       </c>
       <c r="C411" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D411">
         <v>50</v>
@@ -26313,7 +26307,7 @@
         <v>90</v>
       </c>
       <c r="C412" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D412">
         <v>50</v>
@@ -26327,7 +26321,7 @@
         <v>90</v>
       </c>
       <c r="C413" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D413">
         <v>50</v>
@@ -26341,7 +26335,7 @@
         <v>90</v>
       </c>
       <c r="C414" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D414">
         <v>50</v>
@@ -26355,7 +26349,7 @@
         <v>91</v>
       </c>
       <c r="C415" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D415">
         <v>50</v>
@@ -26369,7 +26363,7 @@
         <v>91</v>
       </c>
       <c r="C416" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D416">
         <v>50</v>
@@ -26383,7 +26377,7 @@
         <v>91</v>
       </c>
       <c r="C417" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D417">
         <v>50</v>
@@ -26397,7 +26391,7 @@
         <v>91</v>
       </c>
       <c r="C418" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D418">
         <v>50</v>
@@ -26411,7 +26405,7 @@
         <v>188</v>
       </c>
       <c r="C419" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D419">
         <v>50</v>
@@ -26425,7 +26419,7 @@
         <v>188</v>
       </c>
       <c r="C420" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D420">
         <v>50</v>
@@ -26439,7 +26433,7 @@
         <v>188</v>
       </c>
       <c r="C421" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D421">
         <v>50</v>
@@ -26453,7 +26447,7 @@
         <v>188</v>
       </c>
       <c r="C422" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D422">
         <v>50</v>
@@ -26467,7 +26461,7 @@
         <v>600</v>
       </c>
       <c r="C423" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D423">
         <v>50</v>
@@ -26481,7 +26475,7 @@
         <v>600</v>
       </c>
       <c r="C424" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D424">
         <v>50</v>
@@ -26495,7 +26489,7 @@
         <v>600</v>
       </c>
       <c r="C425" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D425">
         <v>50</v>
@@ -26509,7 +26503,7 @@
         <v>600</v>
       </c>
       <c r="C426" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D426">
         <v>50</v>
@@ -26523,7 +26517,7 @@
         <v>600</v>
       </c>
       <c r="C427" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D427">
         <v>50</v>
@@ -26537,7 +26531,7 @@
         <v>85</v>
       </c>
       <c r="C428" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D428">
         <v>50</v>
@@ -26551,7 +26545,7 @@
         <v>85</v>
       </c>
       <c r="C429" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D429">
         <v>50</v>
@@ -26565,7 +26559,7 @@
         <v>85</v>
       </c>
       <c r="C430" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D430">
         <v>50</v>
@@ -26579,7 +26573,7 @@
         <v>85</v>
       </c>
       <c r="C431" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D431">
         <v>50</v>
@@ -26593,7 +26587,7 @@
         <v>85</v>
       </c>
       <c r="C432" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D432">
         <v>50</v>
@@ -26607,7 +26601,7 @@
         <v>86</v>
       </c>
       <c r="C433" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D433">
         <v>50</v>
@@ -26621,7 +26615,7 @@
         <v>86</v>
       </c>
       <c r="C434" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D434">
         <v>50</v>
@@ -26635,7 +26629,7 @@
         <v>86</v>
       </c>
       <c r="C435" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D435">
         <v>50</v>
@@ -26649,7 +26643,7 @@
         <v>86</v>
       </c>
       <c r="C436" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D436">
         <v>50</v>
@@ -26663,7 +26657,7 @@
         <v>86</v>
       </c>
       <c r="C437" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D437">
         <v>50</v>
@@ -26677,7 +26671,7 @@
         <v>87</v>
       </c>
       <c r="C438" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D438">
         <v>50</v>
@@ -26691,7 +26685,7 @@
         <v>87</v>
       </c>
       <c r="C439" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D439">
         <v>50</v>
@@ -26705,7 +26699,7 @@
         <v>87</v>
       </c>
       <c r="C440" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D440">
         <v>50</v>
@@ -26719,7 +26713,7 @@
         <v>87</v>
       </c>
       <c r="C441" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D441">
         <v>50</v>
@@ -26733,7 +26727,7 @@
         <v>87</v>
       </c>
       <c r="C442" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D442">
         <v>50</v>
@@ -26747,7 +26741,7 @@
         <v>89</v>
       </c>
       <c r="C443" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D443">
         <v>50</v>
@@ -26761,7 +26755,7 @@
         <v>89</v>
       </c>
       <c r="C444" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D444">
         <v>50</v>
@@ -26775,7 +26769,7 @@
         <v>89</v>
       </c>
       <c r="C445" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D445">
         <v>50</v>
@@ -26789,7 +26783,7 @@
         <v>89</v>
       </c>
       <c r="C446" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D446">
         <v>50</v>
@@ -26803,7 +26797,7 @@
         <v>89</v>
       </c>
       <c r="C447" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D447">
         <v>50</v>
@@ -26817,7 +26811,7 @@
         <v>538</v>
       </c>
       <c r="C448" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D448">
         <v>50</v>
@@ -26831,7 +26825,7 @@
         <v>538</v>
       </c>
       <c r="C449" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D449">
         <v>50</v>
@@ -26845,7 +26839,7 @@
         <v>538</v>
       </c>
       <c r="C450" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D450">
         <v>50</v>
@@ -26859,7 +26853,7 @@
         <v>538</v>
       </c>
       <c r="C451" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D451">
         <v>50</v>
@@ -26873,7 +26867,7 @@
         <v>538</v>
       </c>
       <c r="C452" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D452">
         <v>50</v>
@@ -26887,7 +26881,7 @@
         <v>575</v>
       </c>
       <c r="C453" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D453">
         <v>50</v>
@@ -26901,7 +26895,7 @@
         <v>575</v>
       </c>
       <c r="C454" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D454">
         <v>50</v>
@@ -26915,7 +26909,7 @@
         <v>575</v>
       </c>
       <c r="C455" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D455">
         <v>50</v>
@@ -26929,7 +26923,7 @@
         <v>575</v>
       </c>
       <c r="C456" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D456">
         <v>50</v>
@@ -26943,7 +26937,7 @@
         <v>575</v>
       </c>
       <c r="C457" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D457">
         <v>50</v>
@@ -26957,7 +26951,7 @@
         <v>576</v>
       </c>
       <c r="C458" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D458">
         <v>50</v>
@@ -26971,7 +26965,7 @@
         <v>576</v>
       </c>
       <c r="C459" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D459">
         <v>50</v>
@@ -26985,7 +26979,7 @@
         <v>576</v>
       </c>
       <c r="C460" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D460">
         <v>50</v>
@@ -26999,7 +26993,7 @@
         <v>576</v>
       </c>
       <c r="C461" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D461">
         <v>50</v>
@@ -27013,7 +27007,7 @@
         <v>576</v>
       </c>
       <c r="C462" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D462">
         <v>50</v>
@@ -27027,7 +27021,7 @@
         <v>554</v>
       </c>
       <c r="C463" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D463">
         <v>50</v>
@@ -27041,7 +27035,7 @@
         <v>554</v>
       </c>
       <c r="C464" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D464">
         <v>50</v>
@@ -27055,7 +27049,7 @@
         <v>554</v>
       </c>
       <c r="C465" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D465">
         <v>50</v>
@@ -27069,7 +27063,7 @@
         <v>32</v>
       </c>
       <c r="C466" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D466">
         <v>50</v>
@@ -27083,7 +27077,7 @@
         <v>32</v>
       </c>
       <c r="C467" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D467">
         <v>50</v>
@@ -27097,7 +27091,7 @@
         <v>32</v>
       </c>
       <c r="C468" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D468">
         <v>50</v>
@@ -27111,7 +27105,7 @@
         <v>407</v>
       </c>
       <c r="C469" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D469">
         <v>50</v>
@@ -27125,7 +27119,7 @@
         <v>407</v>
       </c>
       <c r="C470" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D470">
         <v>50</v>
@@ -27139,7 +27133,7 @@
         <v>407</v>
       </c>
       <c r="C471" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D471">
         <v>50</v>
@@ -27153,7 +27147,7 @@
         <v>61</v>
       </c>
       <c r="C472" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D472">
         <v>50</v>
@@ -27167,7 +27161,7 @@
         <v>61</v>
       </c>
       <c r="C473" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D473">
         <v>50</v>
@@ -27181,7 +27175,7 @@
         <v>61</v>
       </c>
       <c r="C474" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D474">
         <v>50</v>
@@ -27195,7 +27189,7 @@
         <v>395</v>
       </c>
       <c r="C475" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D475">
         <v>50</v>
@@ -27209,7 +27203,7 @@
         <v>395</v>
       </c>
       <c r="C476" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D476">
         <v>50</v>
@@ -27223,7 +27217,7 @@
         <v>395</v>
       </c>
       <c r="C477" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D477">
         <v>50</v>
@@ -27237,7 +27231,7 @@
         <v>396</v>
       </c>
       <c r="C478" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D478">
         <v>50</v>
@@ -27251,7 +27245,7 @@
         <v>396</v>
       </c>
       <c r="C479" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D479">
         <v>50</v>
@@ -27265,7 +27259,7 @@
         <v>396</v>
       </c>
       <c r="C480" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D480">
         <v>50</v>

</xml_diff>

<commit_message>
check solog size ... (#18)
</commit_message>
<xml_diff>
--- a/database/data_Project_VVIP_Final.xlsx
+++ b/database/data_Project_VVIP_Final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5112"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5112" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4106" uniqueCount="1609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4106" uniqueCount="1607">
   <si>
     <t>Tee Tele Bear</t>
   </si>
@@ -4818,33 +4818,6 @@
     <t>z5404487280405_cd2f69aafada3d2ed353b49b0d6ae01217147288311714728831</t>
   </si>
   <si>
-    <t xml:space="preserve"> S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  L</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  XL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  2XL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  3XL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Freesize</t>
-  </si>
-  <si>
     <t>productStock</t>
   </si>
   <si>
@@ -4852,6 +4825,27 @@
   </si>
   <si>
     <t>productImagesLarge</t>
+  </si>
+  <si>
+    <t>colorId</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>2XL</t>
+  </si>
+  <si>
+    <t>3XL</t>
   </si>
 </sst>
 </file>
@@ -5311,7 +5305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -5360,10 +5354,10 @@
         <v>185</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>1607</v>
+        <v>1598</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>1608</v>
+        <v>1599</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>187</v>
@@ -20540,8 +20534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D480"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -20556,13 +20550,13 @@
         <v>181</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>669</v>
+        <v>1600</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>186</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>1606</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -20573,7 +20567,7 @@
         <v>635</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -20587,7 +20581,7 @@
         <v>635</v>
       </c>
       <c r="C3" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -20601,7 +20595,7 @@
         <v>635</v>
       </c>
       <c r="C4" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -20615,7 +20609,7 @@
         <v>634</v>
       </c>
       <c r="C5" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -20629,7 +20623,7 @@
         <v>634</v>
       </c>
       <c r="C6" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -20643,7 +20637,7 @@
         <v>634</v>
       </c>
       <c r="C7" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -20657,7 +20651,7 @@
         <v>633</v>
       </c>
       <c r="C8" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -20671,7 +20665,7 @@
         <v>633</v>
       </c>
       <c r="C9" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -20685,7 +20679,7 @@
         <v>633</v>
       </c>
       <c r="C10" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D10">
         <v>50</v>
@@ -20699,7 +20693,7 @@
         <v>632</v>
       </c>
       <c r="C11" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -20713,7 +20707,7 @@
         <v>632</v>
       </c>
       <c r="C12" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D12">
         <v>50</v>
@@ -20727,7 +20721,7 @@
         <v>632</v>
       </c>
       <c r="C13" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D13">
         <v>50</v>
@@ -20741,7 +20735,7 @@
         <v>631</v>
       </c>
       <c r="C14" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D14">
         <v>50</v>
@@ -20755,7 +20749,7 @@
         <v>631</v>
       </c>
       <c r="C15" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D15">
         <v>50</v>
@@ -20769,7 +20763,7 @@
         <v>631</v>
       </c>
       <c r="C16" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D16">
         <v>50</v>
@@ -20783,7 +20777,7 @@
         <v>631</v>
       </c>
       <c r="C17" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D17">
         <v>50</v>
@@ -20797,7 +20791,7 @@
         <v>616</v>
       </c>
       <c r="C18" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D18">
         <v>50</v>
@@ -20811,7 +20805,7 @@
         <v>616</v>
       </c>
       <c r="C19" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D19">
         <v>50</v>
@@ -20825,7 +20819,7 @@
         <v>616</v>
       </c>
       <c r="C20" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D20">
         <v>50</v>
@@ -20839,7 +20833,7 @@
         <v>616</v>
       </c>
       <c r="C21" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D21">
         <v>50</v>
@@ -20853,7 +20847,7 @@
         <v>629</v>
       </c>
       <c r="C22" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D22">
         <v>50</v>
@@ -20867,7 +20861,7 @@
         <v>629</v>
       </c>
       <c r="C23" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D23">
         <v>50</v>
@@ -20881,7 +20875,7 @@
         <v>629</v>
       </c>
       <c r="C24" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D24">
         <v>50</v>
@@ -20895,7 +20889,7 @@
         <v>629</v>
       </c>
       <c r="C25" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D25">
         <v>50</v>
@@ -20909,7 +20903,7 @@
         <v>630</v>
       </c>
       <c r="C26" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D26">
         <v>50</v>
@@ -20923,7 +20917,7 @@
         <v>630</v>
       </c>
       <c r="C27" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D27">
         <v>50</v>
@@ -20937,7 +20931,7 @@
         <v>630</v>
       </c>
       <c r="C28" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D28">
         <v>50</v>
@@ -20951,7 +20945,7 @@
         <v>630</v>
       </c>
       <c r="C29" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D29">
         <v>50</v>
@@ -20965,7 +20959,7 @@
         <v>628</v>
       </c>
       <c r="C30" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D30">
         <v>50</v>
@@ -20979,7 +20973,7 @@
         <v>628</v>
       </c>
       <c r="C31" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D31">
         <v>50</v>
@@ -20993,7 +20987,7 @@
         <v>628</v>
       </c>
       <c r="C32" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D32">
         <v>50</v>
@@ -21007,7 +21001,7 @@
         <v>627</v>
       </c>
       <c r="C33" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D33">
         <v>50</v>
@@ -21021,7 +21015,7 @@
         <v>627</v>
       </c>
       <c r="C34" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D34">
         <v>50</v>
@@ -21035,7 +21029,7 @@
         <v>627</v>
       </c>
       <c r="C35" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D35">
         <v>50</v>
@@ -21049,7 +21043,7 @@
         <v>610</v>
       </c>
       <c r="C36" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D36">
         <v>50</v>
@@ -21063,7 +21057,7 @@
         <v>610</v>
       </c>
       <c r="C37" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D37">
         <v>50</v>
@@ -21077,7 +21071,7 @@
         <v>609</v>
       </c>
       <c r="C38" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D38">
         <v>50</v>
@@ -21091,7 +21085,7 @@
         <v>609</v>
       </c>
       <c r="C39" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D39">
         <v>50</v>
@@ -21119,7 +21113,7 @@
         <v>622</v>
       </c>
       <c r="C41" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D41">
         <v>50</v>
@@ -21133,7 +21127,7 @@
         <v>622</v>
       </c>
       <c r="C42" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D42">
         <v>50</v>
@@ -21161,7 +21155,7 @@
         <v>621</v>
       </c>
       <c r="C44" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D44">
         <v>50</v>
@@ -21175,7 +21169,7 @@
         <v>621</v>
       </c>
       <c r="C45" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D45">
         <v>50</v>
@@ -21203,7 +21197,7 @@
         <v>618</v>
       </c>
       <c r="C47" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D47">
         <v>50</v>
@@ -21217,7 +21211,7 @@
         <v>618</v>
       </c>
       <c r="C48" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D48">
         <v>50</v>
@@ -21245,7 +21239,7 @@
         <v>617</v>
       </c>
       <c r="C50" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D50">
         <v>50</v>
@@ -21259,7 +21253,7 @@
         <v>617</v>
       </c>
       <c r="C51" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D51">
         <v>50</v>
@@ -21273,7 +21267,7 @@
         <v>624</v>
       </c>
       <c r="C52" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D52">
         <v>50</v>
@@ -21287,7 +21281,7 @@
         <v>624</v>
       </c>
       <c r="C53" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D53">
         <v>50</v>
@@ -21301,7 +21295,7 @@
         <v>624</v>
       </c>
       <c r="C54" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D54">
         <v>50</v>
@@ -21315,7 +21309,7 @@
         <v>624</v>
       </c>
       <c r="C55" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D55">
         <v>50</v>
@@ -21329,7 +21323,7 @@
         <v>623</v>
       </c>
       <c r="C56" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D56">
         <v>50</v>
@@ -21343,7 +21337,7 @@
         <v>623</v>
       </c>
       <c r="C57" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D57">
         <v>50</v>
@@ -21357,7 +21351,7 @@
         <v>623</v>
       </c>
       <c r="C58" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D58">
         <v>50</v>
@@ -21371,7 +21365,7 @@
         <v>623</v>
       </c>
       <c r="C59" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D59">
         <v>50</v>
@@ -21385,7 +21379,7 @@
         <v>620</v>
       </c>
       <c r="C60" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D60">
         <v>50</v>
@@ -21399,7 +21393,7 @@
         <v>620</v>
       </c>
       <c r="C61" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D61">
         <v>50</v>
@@ -21413,7 +21407,7 @@
         <v>620</v>
       </c>
       <c r="C62" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D62">
         <v>50</v>
@@ -21427,7 +21421,7 @@
         <v>619</v>
       </c>
       <c r="C63" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D63">
         <v>50</v>
@@ -21441,7 +21435,7 @@
         <v>619</v>
       </c>
       <c r="C64" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D64">
         <v>50</v>
@@ -21455,7 +21449,7 @@
         <v>619</v>
       </c>
       <c r="C65" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D65">
         <v>50</v>
@@ -21469,7 +21463,7 @@
         <v>614</v>
       </c>
       <c r="C66" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D66">
         <v>50</v>
@@ -21483,7 +21477,7 @@
         <v>614</v>
       </c>
       <c r="C67" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D67">
         <v>50</v>
@@ -21497,7 +21491,7 @@
         <v>614</v>
       </c>
       <c r="C68" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D68">
         <v>50</v>
@@ -21511,7 +21505,7 @@
         <v>613</v>
       </c>
       <c r="C69" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D69">
         <v>50</v>
@@ -21525,7 +21519,7 @@
         <v>613</v>
       </c>
       <c r="C70" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D70">
         <v>50</v>
@@ -21539,7 +21533,7 @@
         <v>613</v>
       </c>
       <c r="C71" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D71">
         <v>50</v>
@@ -21553,7 +21547,7 @@
         <v>612</v>
       </c>
       <c r="C72" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D72">
         <v>50</v>
@@ -21567,7 +21561,7 @@
         <v>612</v>
       </c>
       <c r="C73" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D73">
         <v>50</v>
@@ -21581,7 +21575,7 @@
         <v>612</v>
       </c>
       <c r="C74" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D74">
         <v>50</v>
@@ -21595,7 +21589,7 @@
         <v>611</v>
       </c>
       <c r="C75" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D75">
         <v>50</v>
@@ -21609,7 +21603,7 @@
         <v>611</v>
       </c>
       <c r="C76" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D76">
         <v>50</v>
@@ -21623,7 +21617,7 @@
         <v>611</v>
       </c>
       <c r="C77" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D77">
         <v>50</v>
@@ -21637,7 +21631,7 @@
         <v>607</v>
       </c>
       <c r="C78" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D78">
         <v>50</v>
@@ -21651,7 +21645,7 @@
         <v>607</v>
       </c>
       <c r="C79" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D79">
         <v>50</v>
@@ -21665,7 +21659,7 @@
         <v>607</v>
       </c>
       <c r="C80" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D80">
         <v>50</v>
@@ -21679,7 +21673,7 @@
         <v>606</v>
       </c>
       <c r="C81" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D81">
         <v>50</v>
@@ -21693,7 +21687,7 @@
         <v>606</v>
       </c>
       <c r="C82" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D82">
         <v>50</v>
@@ -21707,7 +21701,7 @@
         <v>606</v>
       </c>
       <c r="C83" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D83">
         <v>50</v>
@@ -21721,7 +21715,7 @@
         <v>603</v>
       </c>
       <c r="C84" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D84">
         <v>50</v>
@@ -21735,7 +21729,7 @@
         <v>603</v>
       </c>
       <c r="C85" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D85">
         <v>50</v>
@@ -21749,7 +21743,7 @@
         <v>603</v>
       </c>
       <c r="C86" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D86">
         <v>50</v>
@@ -21763,7 +21757,7 @@
         <v>602</v>
       </c>
       <c r="C87" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D87">
         <v>50</v>
@@ -21777,7 +21771,7 @@
         <v>602</v>
       </c>
       <c r="C88" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D88">
         <v>50</v>
@@ -21791,7 +21785,7 @@
         <v>602</v>
       </c>
       <c r="C89" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D89">
         <v>50</v>
@@ -21805,7 +21799,7 @@
         <v>601</v>
       </c>
       <c r="C90" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D90">
         <v>50</v>
@@ -21819,7 +21813,7 @@
         <v>601</v>
       </c>
       <c r="C91" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D91">
         <v>50</v>
@@ -21833,7 +21827,7 @@
         <v>601</v>
       </c>
       <c r="C92" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D92">
         <v>50</v>
@@ -21847,7 +21841,7 @@
         <v>601</v>
       </c>
       <c r="C93" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D93">
         <v>50</v>
@@ -21861,7 +21855,7 @@
         <v>601</v>
       </c>
       <c r="C94" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D94">
         <v>50</v>
@@ -21875,7 +21869,7 @@
         <v>599</v>
       </c>
       <c r="C95" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D95">
         <v>50</v>
@@ -21889,7 +21883,7 @@
         <v>599</v>
       </c>
       <c r="C96" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D96">
         <v>50</v>
@@ -21903,7 +21897,7 @@
         <v>599</v>
       </c>
       <c r="C97" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D97">
         <v>50</v>
@@ -21917,7 +21911,7 @@
         <v>597</v>
       </c>
       <c r="C98" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D98">
         <v>50</v>
@@ -21931,7 +21925,7 @@
         <v>597</v>
       </c>
       <c r="C99" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D99">
         <v>50</v>
@@ -21945,7 +21939,7 @@
         <v>597</v>
       </c>
       <c r="C100" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D100">
         <v>50</v>
@@ -21959,7 +21953,7 @@
         <v>598</v>
       </c>
       <c r="C101" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D101">
         <v>50</v>
@@ -21973,7 +21967,7 @@
         <v>598</v>
       </c>
       <c r="C102" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D102">
         <v>50</v>
@@ -21987,7 +21981,7 @@
         <v>598</v>
       </c>
       <c r="C103" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D103">
         <v>50</v>
@@ -22001,7 +21995,7 @@
         <v>596</v>
       </c>
       <c r="C104" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D104">
         <v>50</v>
@@ -22015,7 +22009,7 @@
         <v>596</v>
       </c>
       <c r="C105" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D105">
         <v>50</v>
@@ -22029,7 +22023,7 @@
         <v>596</v>
       </c>
       <c r="C106" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D106">
         <v>50</v>
@@ -22043,7 +22037,7 @@
         <v>595</v>
       </c>
       <c r="C107" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D107">
         <v>50</v>
@@ -22057,7 +22051,7 @@
         <v>595</v>
       </c>
       <c r="C108" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D108">
         <v>50</v>
@@ -22071,7 +22065,7 @@
         <v>595</v>
       </c>
       <c r="C109" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D109">
         <v>50</v>
@@ -22085,7 +22079,7 @@
         <v>594</v>
       </c>
       <c r="C110" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D110">
         <v>50</v>
@@ -22099,7 +22093,7 @@
         <v>594</v>
       </c>
       <c r="C111" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D111">
         <v>50</v>
@@ -22113,7 +22107,7 @@
         <v>594</v>
       </c>
       <c r="C112" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D112">
         <v>50</v>
@@ -22127,7 +22121,7 @@
         <v>592</v>
       </c>
       <c r="C113" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D113">
         <v>50</v>
@@ -22141,7 +22135,7 @@
         <v>592</v>
       </c>
       <c r="C114" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D114">
         <v>50</v>
@@ -22155,7 +22149,7 @@
         <v>592</v>
       </c>
       <c r="C115" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D115">
         <v>50</v>
@@ -22169,7 +22163,7 @@
         <v>593</v>
       </c>
       <c r="C116" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D116">
         <v>50</v>
@@ -22183,7 +22177,7 @@
         <v>593</v>
       </c>
       <c r="C117" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D117">
         <v>50</v>
@@ -22197,7 +22191,7 @@
         <v>593</v>
       </c>
       <c r="C118" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D118">
         <v>50</v>
@@ -22211,7 +22205,7 @@
         <v>591</v>
       </c>
       <c r="C119" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D119">
         <v>50</v>
@@ -22225,7 +22219,7 @@
         <v>591</v>
       </c>
       <c r="C120" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D120">
         <v>50</v>
@@ -22239,7 +22233,7 @@
         <v>591</v>
       </c>
       <c r="C121" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D121">
         <v>50</v>
@@ -22253,7 +22247,7 @@
         <v>589</v>
       </c>
       <c r="C122" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D122">
         <v>50</v>
@@ -22267,7 +22261,7 @@
         <v>589</v>
       </c>
       <c r="C123" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D123">
         <v>50</v>
@@ -22281,7 +22275,7 @@
         <v>589</v>
       </c>
       <c r="C124" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D124">
         <v>50</v>
@@ -22295,7 +22289,7 @@
         <v>590</v>
       </c>
       <c r="C125" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D125">
         <v>50</v>
@@ -22309,7 +22303,7 @@
         <v>590</v>
       </c>
       <c r="C126" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D126">
         <v>50</v>
@@ -22323,7 +22317,7 @@
         <v>590</v>
       </c>
       <c r="C127" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D127">
         <v>50</v>
@@ -22337,7 +22331,7 @@
         <v>588</v>
       </c>
       <c r="C128" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D128">
         <v>50</v>
@@ -22351,7 +22345,7 @@
         <v>588</v>
       </c>
       <c r="C129" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D129">
         <v>50</v>
@@ -22365,7 +22359,7 @@
         <v>588</v>
       </c>
       <c r="C130" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D130">
         <v>50</v>
@@ -22379,7 +22373,7 @@
         <v>586</v>
       </c>
       <c r="C131" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D131">
         <v>50</v>
@@ -22393,7 +22387,7 @@
         <v>586</v>
       </c>
       <c r="C132" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D132">
         <v>50</v>
@@ -22407,7 +22401,7 @@
         <v>586</v>
       </c>
       <c r="C133" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D133">
         <v>50</v>
@@ -22421,7 +22415,7 @@
         <v>587</v>
       </c>
       <c r="C134" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D134">
         <v>50</v>
@@ -22435,7 +22429,7 @@
         <v>587</v>
       </c>
       <c r="C135" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D135">
         <v>50</v>
@@ -22449,7 +22443,7 @@
         <v>587</v>
       </c>
       <c r="C136" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D136">
         <v>50</v>
@@ -22463,7 +22457,7 @@
         <v>582</v>
       </c>
       <c r="C137" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D137">
         <v>50</v>
@@ -22477,7 +22471,7 @@
         <v>582</v>
       </c>
       <c r="C138" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D138">
         <v>50</v>
@@ -22491,7 +22485,7 @@
         <v>581</v>
       </c>
       <c r="C139" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D139">
         <v>50</v>
@@ -22505,7 +22499,7 @@
         <v>581</v>
       </c>
       <c r="C140" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D140">
         <v>50</v>
@@ -22519,7 +22513,7 @@
         <v>482</v>
       </c>
       <c r="C141" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D141">
         <v>50</v>
@@ -22533,7 +22527,7 @@
         <v>482</v>
       </c>
       <c r="C142" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D142">
         <v>50</v>
@@ -22547,7 +22541,7 @@
         <v>494</v>
       </c>
       <c r="C143" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D143">
         <v>50</v>
@@ -22561,7 +22555,7 @@
         <v>494</v>
       </c>
       <c r="C144" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D144">
         <v>50</v>
@@ -22575,7 +22569,7 @@
         <v>574</v>
       </c>
       <c r="C145" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D145">
         <v>50</v>
@@ -22589,7 +22583,7 @@
         <v>573</v>
       </c>
       <c r="C146" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D146">
         <v>50</v>
@@ -22603,7 +22597,7 @@
         <v>573</v>
       </c>
       <c r="C147" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D147">
         <v>50</v>
@@ -22617,7 +22611,7 @@
         <v>572</v>
       </c>
       <c r="C148" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D148">
         <v>50</v>
@@ -22631,7 +22625,7 @@
         <v>572</v>
       </c>
       <c r="C149" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D149">
         <v>50</v>
@@ -22645,7 +22639,7 @@
         <v>578</v>
       </c>
       <c r="C150" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D150">
         <v>50</v>
@@ -22659,7 +22653,7 @@
         <v>578</v>
       </c>
       <c r="C151" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D151">
         <v>50</v>
@@ -22673,7 +22667,7 @@
         <v>578</v>
       </c>
       <c r="C152" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D152">
         <v>50</v>
@@ -22687,7 +22681,7 @@
         <v>569</v>
       </c>
       <c r="C153" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D153">
         <v>50</v>
@@ -22701,7 +22695,7 @@
         <v>569</v>
       </c>
       <c r="C154" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D154">
         <v>50</v>
@@ -22715,7 +22709,7 @@
         <v>567</v>
       </c>
       <c r="C155" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D155">
         <v>50</v>
@@ -22729,7 +22723,7 @@
         <v>567</v>
       </c>
       <c r="C156" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D156">
         <v>50</v>
@@ -22743,7 +22737,7 @@
         <v>566</v>
       </c>
       <c r="C157" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D157">
         <v>50</v>
@@ -22757,7 +22751,7 @@
         <v>566</v>
       </c>
       <c r="C158" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D158">
         <v>50</v>
@@ -22771,7 +22765,7 @@
         <v>563</v>
       </c>
       <c r="C159" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D159">
         <v>50</v>
@@ -22785,7 +22779,7 @@
         <v>563</v>
       </c>
       <c r="C160" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D160">
         <v>50</v>
@@ -22799,7 +22793,7 @@
         <v>561</v>
       </c>
       <c r="C161" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D161">
         <v>50</v>
@@ -22813,7 +22807,7 @@
         <v>561</v>
       </c>
       <c r="C162" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D162">
         <v>50</v>
@@ -22827,7 +22821,7 @@
         <v>559</v>
       </c>
       <c r="C163" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D163">
         <v>50</v>
@@ -22841,7 +22835,7 @@
         <v>559</v>
       </c>
       <c r="C164" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D164">
         <v>50</v>
@@ -22855,7 +22849,7 @@
         <v>559</v>
       </c>
       <c r="C165" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D165">
         <v>50</v>
@@ -22869,7 +22863,7 @@
         <v>557</v>
       </c>
       <c r="C166" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D166">
         <v>50</v>
@@ -22883,7 +22877,7 @@
         <v>557</v>
       </c>
       <c r="C167" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D167">
         <v>50</v>
@@ -22897,7 +22891,7 @@
         <v>557</v>
       </c>
       <c r="C168" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D168">
         <v>50</v>
@@ -22911,7 +22905,7 @@
         <v>558</v>
       </c>
       <c r="C169" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D169">
         <v>50</v>
@@ -22925,7 +22919,7 @@
         <v>558</v>
       </c>
       <c r="C170" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D170">
         <v>50</v>
@@ -22939,7 +22933,7 @@
         <v>558</v>
       </c>
       <c r="C171" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D171">
         <v>50</v>
@@ -22953,7 +22947,7 @@
         <v>556</v>
       </c>
       <c r="C172" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D172">
         <v>50</v>
@@ -22967,7 +22961,7 @@
         <v>556</v>
       </c>
       <c r="C173" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D173">
         <v>50</v>
@@ -22981,7 +22975,7 @@
         <v>556</v>
       </c>
       <c r="C174" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D174">
         <v>50</v>
@@ -22995,7 +22989,7 @@
         <v>555</v>
       </c>
       <c r="C175" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D175">
         <v>50</v>
@@ -23009,7 +23003,7 @@
         <v>555</v>
       </c>
       <c r="C176" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D176">
         <v>50</v>
@@ -23023,7 +23017,7 @@
         <v>555</v>
       </c>
       <c r="C177" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D177">
         <v>50</v>
@@ -23037,7 +23031,7 @@
         <v>553</v>
       </c>
       <c r="C178" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D178">
         <v>50</v>
@@ -23051,7 +23045,7 @@
         <v>553</v>
       </c>
       <c r="C179" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D179">
         <v>50</v>
@@ -23065,7 +23059,7 @@
         <v>553</v>
       </c>
       <c r="C180" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D180">
         <v>50</v>
@@ -23079,7 +23073,7 @@
         <v>551</v>
       </c>
       <c r="C181" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D181">
         <v>50</v>
@@ -23093,7 +23087,7 @@
         <v>551</v>
       </c>
       <c r="C182" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D182">
         <v>50</v>
@@ -23107,7 +23101,7 @@
         <v>551</v>
       </c>
       <c r="C183" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D183">
         <v>50</v>
@@ -23121,7 +23115,7 @@
         <v>550</v>
       </c>
       <c r="C184" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D184">
         <v>50</v>
@@ -23135,7 +23129,7 @@
         <v>550</v>
       </c>
       <c r="C185" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D185">
         <v>50</v>
@@ -23149,7 +23143,7 @@
         <v>550</v>
       </c>
       <c r="C186" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D186">
         <v>50</v>
@@ -23163,7 +23157,7 @@
         <v>549</v>
       </c>
       <c r="C187" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D187">
         <v>50</v>
@@ -23177,7 +23171,7 @@
         <v>549</v>
       </c>
       <c r="C188" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D188">
         <v>50</v>
@@ -23191,7 +23185,7 @@
         <v>547</v>
       </c>
       <c r="C189" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D189">
         <v>50</v>
@@ -23205,7 +23199,7 @@
         <v>547</v>
       </c>
       <c r="C190" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D190">
         <v>50</v>
@@ -23219,7 +23213,7 @@
         <v>546</v>
       </c>
       <c r="C191" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D191">
         <v>50</v>
@@ -23233,7 +23227,7 @@
         <v>545</v>
       </c>
       <c r="C192" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D192">
         <v>50</v>
@@ -23247,7 +23241,7 @@
         <v>545</v>
       </c>
       <c r="C193" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D193">
         <v>50</v>
@@ -23261,7 +23255,7 @@
         <v>543</v>
       </c>
       <c r="C194" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D194">
         <v>50</v>
@@ -23275,7 +23269,7 @@
         <v>543</v>
       </c>
       <c r="C195" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D195">
         <v>50</v>
@@ -23289,7 +23283,7 @@
         <v>541</v>
       </c>
       <c r="C196" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D196">
         <v>50</v>
@@ -23303,7 +23297,7 @@
         <v>541</v>
       </c>
       <c r="C197" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D197">
         <v>50</v>
@@ -23317,7 +23311,7 @@
         <v>541</v>
       </c>
       <c r="C198" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D198">
         <v>50</v>
@@ -23331,7 +23325,7 @@
         <v>540</v>
       </c>
       <c r="C199" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D199">
         <v>50</v>
@@ -23345,7 +23339,7 @@
         <v>540</v>
       </c>
       <c r="C200" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D200">
         <v>50</v>
@@ -23359,7 +23353,7 @@
         <v>540</v>
       </c>
       <c r="C201" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D201">
         <v>50</v>
@@ -23373,7 +23367,7 @@
         <v>537</v>
       </c>
       <c r="C202" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D202">
         <v>50</v>
@@ -23387,7 +23381,7 @@
         <v>537</v>
       </c>
       <c r="C203" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D203">
         <v>50</v>
@@ -23401,7 +23395,7 @@
         <v>537</v>
       </c>
       <c r="C204" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D204">
         <v>50</v>
@@ -23415,7 +23409,7 @@
         <v>536</v>
       </c>
       <c r="C205" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D205">
         <v>50</v>
@@ -23429,7 +23423,7 @@
         <v>536</v>
       </c>
       <c r="C206" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D206">
         <v>50</v>
@@ -23443,7 +23437,7 @@
         <v>536</v>
       </c>
       <c r="C207" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D207">
         <v>50</v>
@@ -23457,7 +23451,7 @@
         <v>535</v>
       </c>
       <c r="C208" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D208">
         <v>50</v>
@@ -23471,7 +23465,7 @@
         <v>535</v>
       </c>
       <c r="C209" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D209">
         <v>50</v>
@@ -23485,7 +23479,7 @@
         <v>535</v>
       </c>
       <c r="C210" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D210">
         <v>50</v>
@@ -23499,7 +23493,7 @@
         <v>533</v>
       </c>
       <c r="C211" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D211">
         <v>50</v>
@@ -23513,7 +23507,7 @@
         <v>533</v>
       </c>
       <c r="C212" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D212">
         <v>50</v>
@@ -23527,7 +23521,7 @@
         <v>533</v>
       </c>
       <c r="C213" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D213">
         <v>50</v>
@@ -23541,7 +23535,7 @@
         <v>533</v>
       </c>
       <c r="C214" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D214">
         <v>50</v>
@@ -23555,7 +23549,7 @@
         <v>532</v>
       </c>
       <c r="C215" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D215">
         <v>50</v>
@@ -23569,7 +23563,7 @@
         <v>532</v>
       </c>
       <c r="C216" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D216">
         <v>50</v>
@@ -23583,7 +23577,7 @@
         <v>532</v>
       </c>
       <c r="C217" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D217">
         <v>50</v>
@@ -23597,7 +23591,7 @@
         <v>532</v>
       </c>
       <c r="C218" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D218">
         <v>50</v>
@@ -23611,7 +23605,7 @@
         <v>531</v>
       </c>
       <c r="C219" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D219">
         <v>50</v>
@@ -23625,7 +23619,7 @@
         <v>531</v>
       </c>
       <c r="C220" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D220">
         <v>50</v>
@@ -23639,7 +23633,7 @@
         <v>531</v>
       </c>
       <c r="C221" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D221">
         <v>50</v>
@@ -23653,7 +23647,7 @@
         <v>530</v>
       </c>
       <c r="C222" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D222">
         <v>50</v>
@@ -23667,7 +23661,7 @@
         <v>530</v>
       </c>
       <c r="C223" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D223">
         <v>50</v>
@@ -23681,7 +23675,7 @@
         <v>530</v>
       </c>
       <c r="C224" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D224">
         <v>50</v>
@@ -23695,7 +23689,7 @@
         <v>529</v>
       </c>
       <c r="C225" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D225">
         <v>50</v>
@@ -23709,7 +23703,7 @@
         <v>529</v>
       </c>
       <c r="C226" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D226">
         <v>50</v>
@@ -23723,7 +23717,7 @@
         <v>529</v>
       </c>
       <c r="C227" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D227">
         <v>50</v>
@@ -23737,7 +23731,7 @@
         <v>527</v>
       </c>
       <c r="C228" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D228">
         <v>50</v>
@@ -23751,7 +23745,7 @@
         <v>527</v>
       </c>
       <c r="C229" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D229">
         <v>50</v>
@@ -23765,7 +23759,7 @@
         <v>527</v>
       </c>
       <c r="C230" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D230">
         <v>50</v>
@@ -23779,7 +23773,7 @@
         <v>528</v>
       </c>
       <c r="C231" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D231">
         <v>50</v>
@@ -23793,7 +23787,7 @@
         <v>528</v>
       </c>
       <c r="C232" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D232">
         <v>50</v>
@@ -23807,7 +23801,7 @@
         <v>528</v>
       </c>
       <c r="C233" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D233">
         <v>50</v>
@@ -23821,7 +23815,7 @@
         <v>526</v>
       </c>
       <c r="C234" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D234">
         <v>50</v>
@@ -23835,7 +23829,7 @@
         <v>526</v>
       </c>
       <c r="C235" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D235">
         <v>50</v>
@@ -23849,7 +23843,7 @@
         <v>526</v>
       </c>
       <c r="C236" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D236">
         <v>50</v>
@@ -23863,7 +23857,7 @@
         <v>525</v>
       </c>
       <c r="C237" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D237">
         <v>50</v>
@@ -23877,7 +23871,7 @@
         <v>525</v>
       </c>
       <c r="C238" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D238">
         <v>50</v>
@@ -23891,7 +23885,7 @@
         <v>525</v>
       </c>
       <c r="C239" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D239">
         <v>50</v>
@@ -23905,7 +23899,7 @@
         <v>512</v>
       </c>
       <c r="C240" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D240">
         <v>50</v>
@@ -23919,7 +23913,7 @@
         <v>493</v>
       </c>
       <c r="C241" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D241">
         <v>50</v>
@@ -23933,7 +23927,7 @@
         <v>493</v>
       </c>
       <c r="C242" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D242">
         <v>50</v>
@@ -23947,7 +23941,7 @@
         <v>493</v>
       </c>
       <c r="C243" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D243">
         <v>50</v>
@@ -23961,7 +23955,7 @@
         <v>473</v>
       </c>
       <c r="C244" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D244">
         <v>50</v>
@@ -23975,7 +23969,7 @@
         <v>473</v>
       </c>
       <c r="C245" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D245">
         <v>50</v>
@@ -23989,7 +23983,7 @@
         <v>473</v>
       </c>
       <c r="C246" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D246">
         <v>50</v>
@@ -24003,7 +23997,7 @@
         <v>472</v>
       </c>
       <c r="C247" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D247">
         <v>50</v>
@@ -24017,7 +24011,7 @@
         <v>472</v>
       </c>
       <c r="C248" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D248">
         <v>50</v>
@@ -24031,7 +24025,7 @@
         <v>472</v>
       </c>
       <c r="C249" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D249">
         <v>50</v>
@@ -24045,7 +24039,7 @@
         <v>501</v>
       </c>
       <c r="C250" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D250">
         <v>50</v>
@@ -24059,7 +24053,7 @@
         <v>495</v>
       </c>
       <c r="C251" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D251">
         <v>50</v>
@@ -24073,7 +24067,7 @@
         <v>496</v>
       </c>
       <c r="C252" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D252">
         <v>50</v>
@@ -24087,7 +24081,7 @@
         <v>497</v>
       </c>
       <c r="C253" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D253">
         <v>50</v>
@@ -24101,7 +24095,7 @@
         <v>498</v>
       </c>
       <c r="C254" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D254">
         <v>50</v>
@@ -24115,7 +24109,7 @@
         <v>499</v>
       </c>
       <c r="C255" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D255">
         <v>50</v>
@@ -24129,7 +24123,7 @@
         <v>500</v>
       </c>
       <c r="C256" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D256">
         <v>50</v>
@@ -24143,7 +24137,7 @@
         <v>469</v>
       </c>
       <c r="C257" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D257">
         <v>50</v>
@@ -24157,7 +24151,7 @@
         <v>469</v>
       </c>
       <c r="C258" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D258">
         <v>50</v>
@@ -24171,7 +24165,7 @@
         <v>506</v>
       </c>
       <c r="C259" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D259">
         <v>50</v>
@@ -24185,7 +24179,7 @@
         <v>506</v>
       </c>
       <c r="C260" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D260">
         <v>50</v>
@@ -24199,7 +24193,7 @@
         <v>452</v>
       </c>
       <c r="C261" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D261">
         <v>50</v>
@@ -24213,7 +24207,7 @@
         <v>452</v>
       </c>
       <c r="C262" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D262">
         <v>50</v>
@@ -24227,7 +24221,7 @@
         <v>517</v>
       </c>
       <c r="C263" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D263">
         <v>50</v>
@@ -24241,7 +24235,7 @@
         <v>517</v>
       </c>
       <c r="C264" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D264">
         <v>50</v>
@@ -24255,7 +24249,7 @@
         <v>461</v>
       </c>
       <c r="C265" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D265">
         <v>50</v>
@@ -24269,7 +24263,7 @@
         <v>461</v>
       </c>
       <c r="C266" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D266">
         <v>50</v>
@@ -24283,7 +24277,7 @@
         <v>508</v>
       </c>
       <c r="C267" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D267">
         <v>50</v>
@@ -24297,7 +24291,7 @@
         <v>508</v>
       </c>
       <c r="C268" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D268">
         <v>50</v>
@@ -24311,7 +24305,7 @@
         <v>470</v>
       </c>
       <c r="C269" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D269">
         <v>50</v>
@@ -24325,7 +24319,7 @@
         <v>470</v>
       </c>
       <c r="C270" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D270">
         <v>50</v>
@@ -24339,7 +24333,7 @@
         <v>484</v>
       </c>
       <c r="C271" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D271">
         <v>50</v>
@@ -24353,7 +24347,7 @@
         <v>484</v>
       </c>
       <c r="C272" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D272">
         <v>50</v>
@@ -24367,7 +24361,7 @@
         <v>484</v>
       </c>
       <c r="C273" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D273">
         <v>50</v>
@@ -24381,7 +24375,7 @@
         <v>476</v>
       </c>
       <c r="C274" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D274">
         <v>50</v>
@@ -24395,7 +24389,7 @@
         <v>476</v>
       </c>
       <c r="C275" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D275">
         <v>50</v>
@@ -24409,7 +24403,7 @@
         <v>462</v>
       </c>
       <c r="C276" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D276">
         <v>50</v>
@@ -24423,7 +24417,7 @@
         <v>462</v>
       </c>
       <c r="C277" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D277">
         <v>50</v>
@@ -24437,7 +24431,7 @@
         <v>463</v>
       </c>
       <c r="C278" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D278">
         <v>50</v>
@@ -24451,7 +24445,7 @@
         <v>463</v>
       </c>
       <c r="C279" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D279">
         <v>50</v>
@@ -24465,7 +24459,7 @@
         <v>455</v>
       </c>
       <c r="C280" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D280">
         <v>50</v>
@@ -24479,7 +24473,7 @@
         <v>455</v>
       </c>
       <c r="C281" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D281">
         <v>50</v>
@@ -24493,7 +24487,7 @@
         <v>456</v>
       </c>
       <c r="C282" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D282">
         <v>50</v>
@@ -24507,7 +24501,7 @@
         <v>456</v>
       </c>
       <c r="C283" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D283">
         <v>50</v>
@@ -24521,7 +24515,7 @@
         <v>218</v>
       </c>
       <c r="C284" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D284">
         <v>50</v>
@@ -24535,7 +24529,7 @@
         <v>218</v>
       </c>
       <c r="C285" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D285">
         <v>50</v>
@@ -24549,7 +24543,7 @@
         <v>460</v>
       </c>
       <c r="C286" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D286">
         <v>50</v>
@@ -24563,7 +24557,7 @@
         <v>460</v>
       </c>
       <c r="C287" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D287">
         <v>50</v>
@@ -24577,7 +24571,7 @@
         <v>445</v>
       </c>
       <c r="C288" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D288">
         <v>50</v>
@@ -24591,7 +24585,7 @@
         <v>445</v>
       </c>
       <c r="C289" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D289">
         <v>50</v>
@@ -24605,7 +24599,7 @@
         <v>404</v>
       </c>
       <c r="C290" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D290">
         <v>50</v>
@@ -24619,7 +24613,7 @@
         <v>404</v>
       </c>
       <c r="C291" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D291">
         <v>50</v>
@@ -24633,7 +24627,7 @@
         <v>404</v>
       </c>
       <c r="C292" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D292">
         <v>50</v>
@@ -24647,7 +24641,7 @@
         <v>403</v>
       </c>
       <c r="C293" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D293">
         <v>50</v>
@@ -24661,7 +24655,7 @@
         <v>403</v>
       </c>
       <c r="C294" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D294">
         <v>50</v>
@@ -24675,7 +24669,7 @@
         <v>403</v>
       </c>
       <c r="C295" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D295">
         <v>50</v>
@@ -24689,7 +24683,7 @@
         <v>405</v>
       </c>
       <c r="C296" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D296">
         <v>50</v>
@@ -24703,7 +24697,7 @@
         <v>451</v>
       </c>
       <c r="C297" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D297">
         <v>50</v>
@@ -24717,7 +24711,7 @@
         <v>451</v>
       </c>
       <c r="C298" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D298">
         <v>50</v>
@@ -24731,7 +24725,7 @@
         <v>451</v>
       </c>
       <c r="C299" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D299">
         <v>50</v>
@@ -24745,7 +24739,7 @@
         <v>449</v>
       </c>
       <c r="C300" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D300">
         <v>50</v>
@@ -24759,7 +24753,7 @@
         <v>449</v>
       </c>
       <c r="C301" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D301">
         <v>50</v>
@@ -24773,7 +24767,7 @@
         <v>449</v>
       </c>
       <c r="C302" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D302">
         <v>50</v>
@@ -24787,7 +24781,7 @@
         <v>450</v>
       </c>
       <c r="C303" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D303">
         <v>50</v>
@@ -24801,7 +24795,7 @@
         <v>450</v>
       </c>
       <c r="C304" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D304">
         <v>50</v>
@@ -24815,7 +24809,7 @@
         <v>450</v>
       </c>
       <c r="C305" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D305">
         <v>50</v>
@@ -24829,7 +24823,7 @@
         <v>468</v>
       </c>
       <c r="C306" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D306">
         <v>50</v>
@@ -24843,7 +24837,7 @@
         <v>468</v>
       </c>
       <c r="C307" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D307">
         <v>50</v>
@@ -24857,7 +24851,7 @@
         <v>468</v>
       </c>
       <c r="C308" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D308">
         <v>50</v>
@@ -24871,7 +24865,7 @@
         <v>319</v>
       </c>
       <c r="C309" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D309">
         <v>50</v>
@@ -24885,7 +24879,7 @@
         <v>319</v>
       </c>
       <c r="C310" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D310">
         <v>50</v>
@@ -24899,7 +24893,7 @@
         <v>319</v>
       </c>
       <c r="C311" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D311">
         <v>50</v>
@@ -24913,7 +24907,7 @@
         <v>321</v>
       </c>
       <c r="C312" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D312">
         <v>50</v>
@@ -24927,7 +24921,7 @@
         <v>321</v>
       </c>
       <c r="C313" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D313">
         <v>50</v>
@@ -24941,7 +24935,7 @@
         <v>321</v>
       </c>
       <c r="C314" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D314">
         <v>50</v>
@@ -24955,7 +24949,7 @@
         <v>364</v>
       </c>
       <c r="C315" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D315">
         <v>50</v>
@@ -24969,7 +24963,7 @@
         <v>364</v>
       </c>
       <c r="C316" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D316">
         <v>50</v>
@@ -24983,7 +24977,7 @@
         <v>364</v>
       </c>
       <c r="C317" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D317">
         <v>50</v>
@@ -24997,7 +24991,7 @@
         <v>338</v>
       </c>
       <c r="C318" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D318">
         <v>50</v>
@@ -25011,7 +25005,7 @@
         <v>338</v>
       </c>
       <c r="C319" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D319">
         <v>50</v>
@@ -25025,7 +25019,7 @@
         <v>338</v>
       </c>
       <c r="C320" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D320">
         <v>50</v>
@@ -25039,7 +25033,7 @@
         <v>338</v>
       </c>
       <c r="C321" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D321">
         <v>50</v>
@@ -25053,7 +25047,7 @@
         <v>93</v>
       </c>
       <c r="C322" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D322">
         <v>50</v>
@@ -25067,7 +25061,7 @@
         <v>93</v>
       </c>
       <c r="C323" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D323">
         <v>50</v>
@@ -25081,7 +25075,7 @@
         <v>93</v>
       </c>
       <c r="C324" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D324">
         <v>50</v>
@@ -25095,7 +25089,7 @@
         <v>93</v>
       </c>
       <c r="C325" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D325">
         <v>50</v>
@@ -25109,7 +25103,7 @@
         <v>95</v>
       </c>
       <c r="C326" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D326">
         <v>50</v>
@@ -25123,7 +25117,7 @@
         <v>95</v>
       </c>
       <c r="C327" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D327">
         <v>50</v>
@@ -25137,7 +25131,7 @@
         <v>95</v>
       </c>
       <c r="C328" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D328">
         <v>50</v>
@@ -25151,7 +25145,7 @@
         <v>95</v>
       </c>
       <c r="C329" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D329">
         <v>50</v>
@@ -25165,7 +25159,7 @@
         <v>73</v>
       </c>
       <c r="C330" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D330">
         <v>50</v>
@@ -25179,7 +25173,7 @@
         <v>73</v>
       </c>
       <c r="C331" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D331">
         <v>50</v>
@@ -25193,7 +25187,7 @@
         <v>73</v>
       </c>
       <c r="C332" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D332">
         <v>50</v>
@@ -25207,7 +25201,7 @@
         <v>73</v>
       </c>
       <c r="C333" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D333">
         <v>50</v>
@@ -25221,7 +25215,7 @@
         <v>71</v>
       </c>
       <c r="C334" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D334">
         <v>50</v>
@@ -25235,7 +25229,7 @@
         <v>71</v>
       </c>
       <c r="C335" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D335">
         <v>50</v>
@@ -25249,7 +25243,7 @@
         <v>71</v>
       </c>
       <c r="C336" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D336">
         <v>50</v>
@@ -25263,7 +25257,7 @@
         <v>71</v>
       </c>
       <c r="C337" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D337">
         <v>50</v>
@@ -25277,7 +25271,7 @@
         <v>72</v>
       </c>
       <c r="C338" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D338">
         <v>50</v>
@@ -25291,7 +25285,7 @@
         <v>72</v>
       </c>
       <c r="C339" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D339">
         <v>50</v>
@@ -25305,7 +25299,7 @@
         <v>72</v>
       </c>
       <c r="C340" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D340">
         <v>50</v>
@@ -25319,7 +25313,7 @@
         <v>72</v>
       </c>
       <c r="C341" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D341">
         <v>50</v>
@@ -25333,7 +25327,7 @@
         <v>480</v>
       </c>
       <c r="C342" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D342">
         <v>50</v>
@@ -25347,7 +25341,7 @@
         <v>480</v>
       </c>
       <c r="C343" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D343">
         <v>50</v>
@@ -25361,7 +25355,7 @@
         <v>480</v>
       </c>
       <c r="C344" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D344">
         <v>50</v>
@@ -25375,7 +25369,7 @@
         <v>480</v>
       </c>
       <c r="C345" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D345">
         <v>50</v>
@@ -25389,7 +25383,7 @@
         <v>325</v>
       </c>
       <c r="C346" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D346">
         <v>50</v>
@@ -25403,7 +25397,7 @@
         <v>325</v>
       </c>
       <c r="C347" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D347">
         <v>50</v>
@@ -25417,7 +25411,7 @@
         <v>325</v>
       </c>
       <c r="C348" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D348">
         <v>50</v>
@@ -25431,7 +25425,7 @@
         <v>325</v>
       </c>
       <c r="C349" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D349">
         <v>50</v>
@@ -25445,7 +25439,7 @@
         <v>256</v>
       </c>
       <c r="C350" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D350">
         <v>50</v>
@@ -25459,7 +25453,7 @@
         <v>256</v>
       </c>
       <c r="C351" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D351">
         <v>50</v>
@@ -25473,7 +25467,7 @@
         <v>256</v>
       </c>
       <c r="C352" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D352">
         <v>50</v>
@@ -25487,7 +25481,7 @@
         <v>256</v>
       </c>
       <c r="C353" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D353">
         <v>50</v>
@@ -25501,7 +25495,7 @@
         <v>257</v>
       </c>
       <c r="C354" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D354">
         <v>50</v>
@@ -25515,7 +25509,7 @@
         <v>257</v>
       </c>
       <c r="C355" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D355">
         <v>50</v>
@@ -25529,7 +25523,7 @@
         <v>257</v>
       </c>
       <c r="C356" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D356">
         <v>50</v>
@@ -25543,7 +25537,7 @@
         <v>257</v>
       </c>
       <c r="C357" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D357">
         <v>50</v>
@@ -25557,7 +25551,7 @@
         <v>327</v>
       </c>
       <c r="C358" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D358">
         <v>50</v>
@@ -25571,7 +25565,7 @@
         <v>327</v>
       </c>
       <c r="C359" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D359">
         <v>50</v>
@@ -25585,7 +25579,7 @@
         <v>327</v>
       </c>
       <c r="C360" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D360">
         <v>50</v>
@@ -25599,7 +25593,7 @@
         <v>327</v>
       </c>
       <c r="C361" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D361">
         <v>50</v>
@@ -25613,7 +25607,7 @@
         <v>326</v>
       </c>
       <c r="C362" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D362">
         <v>50</v>
@@ -25627,7 +25621,7 @@
         <v>326</v>
       </c>
       <c r="C363" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D363">
         <v>50</v>
@@ -25641,7 +25635,7 @@
         <v>326</v>
       </c>
       <c r="C364" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D364">
         <v>50</v>
@@ -25655,7 +25649,7 @@
         <v>326</v>
       </c>
       <c r="C365" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D365">
         <v>50</v>
@@ -25669,7 +25663,7 @@
         <v>310</v>
       </c>
       <c r="C366" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D366">
         <v>50</v>
@@ -25683,7 +25677,7 @@
         <v>278</v>
       </c>
       <c r="C367" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D367">
         <v>50</v>
@@ -25697,7 +25691,7 @@
         <v>322</v>
       </c>
       <c r="C368" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D368">
         <v>50</v>
@@ -25711,7 +25705,7 @@
         <v>311</v>
       </c>
       <c r="C369" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D369">
         <v>50</v>
@@ -25725,7 +25719,7 @@
         <v>299</v>
       </c>
       <c r="C370" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D370">
         <v>50</v>
@@ -25739,7 +25733,7 @@
         <v>299</v>
       </c>
       <c r="C371" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D371">
         <v>50</v>
@@ -25753,7 +25747,7 @@
         <v>299</v>
       </c>
       <c r="C372" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D372">
         <v>50</v>
@@ -25767,7 +25761,7 @@
         <v>299</v>
       </c>
       <c r="C373" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D373">
         <v>50</v>
@@ -25781,7 +25775,7 @@
         <v>274</v>
       </c>
       <c r="C374" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D374">
         <v>50</v>
@@ -25795,7 +25789,7 @@
         <v>274</v>
       </c>
       <c r="C375" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D375">
         <v>50</v>
@@ -25809,7 +25803,7 @@
         <v>274</v>
       </c>
       <c r="C376" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D376">
         <v>50</v>
@@ -25823,7 +25817,7 @@
         <v>274</v>
       </c>
       <c r="C377" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D377">
         <v>50</v>
@@ -25837,7 +25831,7 @@
         <v>272</v>
       </c>
       <c r="C378" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D378">
         <v>50</v>
@@ -25851,7 +25845,7 @@
         <v>272</v>
       </c>
       <c r="C379" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D379">
         <v>50</v>
@@ -25865,7 +25859,7 @@
         <v>272</v>
       </c>
       <c r="C380" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D380">
         <v>50</v>
@@ -25879,7 +25873,7 @@
         <v>272</v>
       </c>
       <c r="C381" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D381">
         <v>50</v>
@@ -25893,7 +25887,7 @@
         <v>273</v>
       </c>
       <c r="C382" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D382">
         <v>50</v>
@@ -25907,7 +25901,7 @@
         <v>273</v>
       </c>
       <c r="C383" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D383">
         <v>50</v>
@@ -25921,7 +25915,7 @@
         <v>273</v>
       </c>
       <c r="C384" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D384">
         <v>50</v>
@@ -25935,7 +25929,7 @@
         <v>273</v>
       </c>
       <c r="C385" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D385">
         <v>50</v>
@@ -25949,7 +25943,7 @@
         <v>229</v>
       </c>
       <c r="C386" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D386">
         <v>50</v>
@@ -25963,7 +25957,7 @@
         <v>229</v>
       </c>
       <c r="C387" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D387">
         <v>50</v>
@@ -25977,7 +25971,7 @@
         <v>229</v>
       </c>
       <c r="C388" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D388">
         <v>50</v>
@@ -25991,7 +25985,7 @@
         <v>229</v>
       </c>
       <c r="C389" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D389">
         <v>50</v>
@@ -26005,7 +25999,7 @@
         <v>160</v>
       </c>
       <c r="C390" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D390">
         <v>50</v>
@@ -26019,7 +26013,7 @@
         <v>159</v>
       </c>
       <c r="C391" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D391">
         <v>50</v>
@@ -26033,7 +26027,7 @@
         <v>158</v>
       </c>
       <c r="C392" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D392">
         <v>50</v>
@@ -26047,7 +26041,7 @@
         <v>157</v>
       </c>
       <c r="C393" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D393">
         <v>50</v>
@@ -26061,7 +26055,7 @@
         <v>298</v>
       </c>
       <c r="C394" t="s">
-        <v>1605</v>
+        <v>394</v>
       </c>
       <c r="D394">
         <v>50</v>
@@ -26075,7 +26069,7 @@
         <v>302</v>
       </c>
       <c r="C395" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D395">
         <v>50</v>
@@ -26089,7 +26083,7 @@
         <v>302</v>
       </c>
       <c r="C396" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D396">
         <v>50</v>
@@ -26103,7 +26097,7 @@
         <v>302</v>
       </c>
       <c r="C397" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D397">
         <v>50</v>
@@ -26117,7 +26111,7 @@
         <v>302</v>
       </c>
       <c r="C398" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D398">
         <v>50</v>
@@ -26131,7 +26125,7 @@
         <v>101</v>
       </c>
       <c r="C399" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D399">
         <v>50</v>
@@ -26145,7 +26139,7 @@
         <v>101</v>
       </c>
       <c r="C400" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D400">
         <v>50</v>
@@ -26159,7 +26153,7 @@
         <v>101</v>
       </c>
       <c r="C401" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D401">
         <v>50</v>
@@ -26173,7 +26167,7 @@
         <v>101</v>
       </c>
       <c r="C402" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D402">
         <v>50</v>
@@ -26187,7 +26181,7 @@
         <v>102</v>
       </c>
       <c r="C403" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D403">
         <v>50</v>
@@ -26201,7 +26195,7 @@
         <v>102</v>
       </c>
       <c r="C404" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D404">
         <v>50</v>
@@ -26215,7 +26209,7 @@
         <v>102</v>
       </c>
       <c r="C405" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D405">
         <v>50</v>
@@ -26229,7 +26223,7 @@
         <v>102</v>
       </c>
       <c r="C406" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D406">
         <v>50</v>
@@ -26243,7 +26237,7 @@
         <v>474</v>
       </c>
       <c r="C407" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D407">
         <v>50</v>
@@ -26257,7 +26251,7 @@
         <v>474</v>
       </c>
       <c r="C408" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D408">
         <v>50</v>
@@ -26271,7 +26265,7 @@
         <v>474</v>
       </c>
       <c r="C409" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D409">
         <v>50</v>
@@ -26285,7 +26279,7 @@
         <v>474</v>
       </c>
       <c r="C410" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D410">
         <v>50</v>
@@ -26299,7 +26293,7 @@
         <v>90</v>
       </c>
       <c r="C411" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D411">
         <v>50</v>
@@ -26313,7 +26307,7 @@
         <v>90</v>
       </c>
       <c r="C412" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D412">
         <v>50</v>
@@ -26327,7 +26321,7 @@
         <v>90</v>
       </c>
       <c r="C413" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D413">
         <v>50</v>
@@ -26341,7 +26335,7 @@
         <v>90</v>
       </c>
       <c r="C414" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D414">
         <v>50</v>
@@ -26355,7 +26349,7 @@
         <v>91</v>
       </c>
       <c r="C415" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D415">
         <v>50</v>
@@ -26369,7 +26363,7 @@
         <v>91</v>
       </c>
       <c r="C416" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D416">
         <v>50</v>
@@ -26383,7 +26377,7 @@
         <v>91</v>
       </c>
       <c r="C417" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D417">
         <v>50</v>
@@ -26397,7 +26391,7 @@
         <v>91</v>
       </c>
       <c r="C418" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D418">
         <v>50</v>
@@ -26411,7 +26405,7 @@
         <v>188</v>
       </c>
       <c r="C419" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D419">
         <v>50</v>
@@ -26425,7 +26419,7 @@
         <v>188</v>
       </c>
       <c r="C420" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D420">
         <v>50</v>
@@ -26439,7 +26433,7 @@
         <v>188</v>
       </c>
       <c r="C421" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D421">
         <v>50</v>
@@ -26453,7 +26447,7 @@
         <v>188</v>
       </c>
       <c r="C422" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D422">
         <v>50</v>
@@ -26467,7 +26461,7 @@
         <v>600</v>
       </c>
       <c r="C423" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D423">
         <v>50</v>
@@ -26481,7 +26475,7 @@
         <v>600</v>
       </c>
       <c r="C424" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D424">
         <v>50</v>
@@ -26495,7 +26489,7 @@
         <v>600</v>
       </c>
       <c r="C425" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D425">
         <v>50</v>
@@ -26509,7 +26503,7 @@
         <v>600</v>
       </c>
       <c r="C426" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D426">
         <v>50</v>
@@ -26523,7 +26517,7 @@
         <v>600</v>
       </c>
       <c r="C427" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D427">
         <v>50</v>
@@ -26537,7 +26531,7 @@
         <v>85</v>
       </c>
       <c r="C428" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D428">
         <v>50</v>
@@ -26551,7 +26545,7 @@
         <v>85</v>
       </c>
       <c r="C429" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D429">
         <v>50</v>
@@ -26565,7 +26559,7 @@
         <v>85</v>
       </c>
       <c r="C430" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D430">
         <v>50</v>
@@ -26579,7 +26573,7 @@
         <v>85</v>
       </c>
       <c r="C431" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D431">
         <v>50</v>
@@ -26593,7 +26587,7 @@
         <v>85</v>
       </c>
       <c r="C432" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D432">
         <v>50</v>
@@ -26607,7 +26601,7 @@
         <v>86</v>
       </c>
       <c r="C433" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D433">
         <v>50</v>
@@ -26621,7 +26615,7 @@
         <v>86</v>
       </c>
       <c r="C434" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D434">
         <v>50</v>
@@ -26635,7 +26629,7 @@
         <v>86</v>
       </c>
       <c r="C435" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D435">
         <v>50</v>
@@ -26649,7 +26643,7 @@
         <v>86</v>
       </c>
       <c r="C436" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D436">
         <v>50</v>
@@ -26663,7 +26657,7 @@
         <v>86</v>
       </c>
       <c r="C437" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D437">
         <v>50</v>
@@ -26677,7 +26671,7 @@
         <v>87</v>
       </c>
       <c r="C438" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D438">
         <v>50</v>
@@ -26691,7 +26685,7 @@
         <v>87</v>
       </c>
       <c r="C439" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D439">
         <v>50</v>
@@ -26705,7 +26699,7 @@
         <v>87</v>
       </c>
       <c r="C440" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D440">
         <v>50</v>
@@ -26719,7 +26713,7 @@
         <v>87</v>
       </c>
       <c r="C441" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D441">
         <v>50</v>
@@ -26733,7 +26727,7 @@
         <v>87</v>
       </c>
       <c r="C442" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D442">
         <v>50</v>
@@ -26747,7 +26741,7 @@
         <v>89</v>
       </c>
       <c r="C443" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D443">
         <v>50</v>
@@ -26761,7 +26755,7 @@
         <v>89</v>
       </c>
       <c r="C444" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D444">
         <v>50</v>
@@ -26775,7 +26769,7 @@
         <v>89</v>
       </c>
       <c r="C445" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D445">
         <v>50</v>
@@ -26789,7 +26783,7 @@
         <v>89</v>
       </c>
       <c r="C446" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D446">
         <v>50</v>
@@ -26803,7 +26797,7 @@
         <v>89</v>
       </c>
       <c r="C447" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D447">
         <v>50</v>
@@ -26817,7 +26811,7 @@
         <v>538</v>
       </c>
       <c r="C448" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D448">
         <v>50</v>
@@ -26831,7 +26825,7 @@
         <v>538</v>
       </c>
       <c r="C449" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D449">
         <v>50</v>
@@ -26845,7 +26839,7 @@
         <v>538</v>
       </c>
       <c r="C450" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D450">
         <v>50</v>
@@ -26859,7 +26853,7 @@
         <v>538</v>
       </c>
       <c r="C451" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D451">
         <v>50</v>
@@ -26873,7 +26867,7 @@
         <v>538</v>
       </c>
       <c r="C452" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D452">
         <v>50</v>
@@ -26887,7 +26881,7 @@
         <v>575</v>
       </c>
       <c r="C453" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D453">
         <v>50</v>
@@ -26901,7 +26895,7 @@
         <v>575</v>
       </c>
       <c r="C454" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D454">
         <v>50</v>
@@ -26915,7 +26909,7 @@
         <v>575</v>
       </c>
       <c r="C455" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D455">
         <v>50</v>
@@ -26929,7 +26923,7 @@
         <v>575</v>
       </c>
       <c r="C456" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D456">
         <v>50</v>
@@ -26943,7 +26937,7 @@
         <v>575</v>
       </c>
       <c r="C457" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D457">
         <v>50</v>
@@ -26957,7 +26951,7 @@
         <v>576</v>
       </c>
       <c r="C458" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
       <c r="D458">
         <v>50</v>
@@ -26971,7 +26965,7 @@
         <v>576</v>
       </c>
       <c r="C459" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D459">
         <v>50</v>
@@ -26985,7 +26979,7 @@
         <v>576</v>
       </c>
       <c r="C460" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="D460">
         <v>50</v>
@@ -26999,7 +26993,7 @@
         <v>576</v>
       </c>
       <c r="C461" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="D461">
         <v>50</v>
@@ -27013,7 +27007,7 @@
         <v>576</v>
       </c>
       <c r="C462" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D462">
         <v>50</v>
@@ -27027,7 +27021,7 @@
         <v>554</v>
       </c>
       <c r="C463" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D463">
         <v>50</v>
@@ -27041,7 +27035,7 @@
         <v>554</v>
       </c>
       <c r="C464" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D464">
         <v>50</v>
@@ -27055,7 +27049,7 @@
         <v>554</v>
       </c>
       <c r="C465" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D465">
         <v>50</v>
@@ -27069,7 +27063,7 @@
         <v>32</v>
       </c>
       <c r="C466" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D466">
         <v>50</v>
@@ -27083,7 +27077,7 @@
         <v>32</v>
       </c>
       <c r="C467" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D467">
         <v>50</v>
@@ -27097,7 +27091,7 @@
         <v>32</v>
       </c>
       <c r="C468" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D468">
         <v>50</v>
@@ -27111,7 +27105,7 @@
         <v>407</v>
       </c>
       <c r="C469" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D469">
         <v>50</v>
@@ -27125,7 +27119,7 @@
         <v>407</v>
       </c>
       <c r="C470" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D470">
         <v>50</v>
@@ -27139,7 +27133,7 @@
         <v>407</v>
       </c>
       <c r="C471" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D471">
         <v>50</v>
@@ -27153,7 +27147,7 @@
         <v>61</v>
       </c>
       <c r="C472" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D472">
         <v>50</v>
@@ -27167,7 +27161,7 @@
         <v>61</v>
       </c>
       <c r="C473" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D473">
         <v>50</v>
@@ -27181,7 +27175,7 @@
         <v>61</v>
       </c>
       <c r="C474" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D474">
         <v>50</v>
@@ -27195,7 +27189,7 @@
         <v>395</v>
       </c>
       <c r="C475" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D475">
         <v>50</v>
@@ -27209,7 +27203,7 @@
         <v>395</v>
       </c>
       <c r="C476" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D476">
         <v>50</v>
@@ -27223,7 +27217,7 @@
         <v>395</v>
       </c>
       <c r="C477" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D477">
         <v>50</v>
@@ -27237,7 +27231,7 @@
         <v>396</v>
       </c>
       <c r="C478" t="s">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="D478">
         <v>50</v>
@@ -27251,7 +27245,7 @@
         <v>396</v>
       </c>
       <c r="C479" t="s">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="D479">
         <v>50</v>
@@ -27265,7 +27259,7 @@
         <v>396</v>
       </c>
       <c r="C480" t="s">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="D480">
         <v>50</v>

</xml_diff>